<commit_message>
Display Records, Fields, and Tables
</commit_message>
<xml_diff>
--- a/3.VisualForce/1.Visualforce-Basics/1.Visualforce-Basics.xlsx
+++ b/3.VisualForce/1.Visualforce-Basics/1.Visualforce-Basics.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\quang\salesforce-trailhead\3.VisualForce\1.Visualforce-Basics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2041F852-2710-4BE0-946A-6B99D53D3D3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{606D40BA-65D2-470C-B2F7-A2BE9DEB8C1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Create And Edit Visualforce Pag" sheetId="1" r:id="rId1"/>
     <sheet name="UseSimpleVariablesAndFormulas" sheetId="2" r:id="rId2"/>
     <sheet name="Use Standard Controllers" sheetId="3" r:id="rId3"/>
+    <sheet name="DisplayRecordsFieldsAndTables" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="49">
   <si>
     <t>DisplayImage</t>
     <phoneticPr fontId="1"/>
@@ -164,9 +165,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>&lt;apex:page standardController="Contact"&gt;</t>
-  </si>
-  <si>
     <t xml:space="preserve">    &lt;apex:pageBlock title="Contact Summary"&gt;</t>
   </si>
   <si>
@@ -183,6 +181,84 @@
   </si>
   <si>
     <t>ContactView</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Display Records, Fields, and Tables</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>https://trailhead.salesforce.com/content/learn/modules/visualforce_fundamentals/visualforce_output_components</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>OppView</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">&lt;apex:page </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Yu Gothic"/>
+        <family val="3"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>standardController="Contact"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">    &lt;apex:outputField value="{! Opportunity.Name }"/&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    &lt;apex:outputField value="{! Opportunity.Amount }"/&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    &lt;apex:outputField value="{! Opportunity.CloseDate }"/&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    &lt;apex:outputField value="{! Opportunity.Account.Name }"/&gt;</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">&lt;apex:page </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Yu Gothic"/>
+        <family val="3"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>name="OppView" standardController="Opportunity"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -190,7 +266,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -211,6 +287,13 @@
       <name val="Yu Gothic"/>
       <family val="3"/>
       <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Yu Gothic"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -320,7 +403,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -333,6 +416,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
@@ -1421,6 +1506,231 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>372869</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>27214</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="図 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9A201CD0-8DAF-20FD-03D6-467CF17F38B1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="814614" y="1021443"/>
+          <a:ext cx="12140326" cy="6943271"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>226786</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>117928</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>88500</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>53642</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="図 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{30664A5B-EF1C-343F-FFE0-8BB037B6410D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="889000" y="8282214"/>
+          <a:ext cx="10457143" cy="6285714"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>90714</xdr:colOff>
+      <xdr:row>67</xdr:row>
+      <xdr:rowOff>72571</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>331404</xdr:colOff>
+      <xdr:row>77</xdr:row>
+      <xdr:rowOff>4714</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="図 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6E60D8D4-57B4-78B5-95D8-E874A906EB52}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1415143" y="15267214"/>
+          <a:ext cx="4876190" cy="2200000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>254000</xdr:colOff>
+      <xdr:row>89</xdr:row>
+      <xdr:rowOff>136071</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>290286</xdr:colOff>
+      <xdr:row>124</xdr:row>
+      <xdr:rowOff>43766</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="図 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{101323BF-C17A-5EC7-F3FD-D5366C2C38A3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="916214" y="20320000"/>
+          <a:ext cx="11956143" cy="7845195"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>125</xdr:row>
+      <xdr:rowOff>127001</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>254000</xdr:colOff>
+      <xdr:row>148</xdr:row>
+      <xdr:rowOff>194689</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="図 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1D58628B-20AB-5473-6CB7-731FEE315B16}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="857250" y="27908251"/>
+          <a:ext cx="12065000" cy="5179438"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -1686,8 +1996,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:T108"/>
   <sheetViews>
-    <sheetView topLeftCell="A133" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="O80" sqref="O80"/>
+    <sheetView topLeftCell="A64" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C79" sqref="C79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18"/>
@@ -1812,7 +2122,7 @@
     </row>
     <row r="79" spans="2:20">
       <c r="B79" s="4"/>
-      <c r="C79" s="4" t="s">
+      <c r="C79" s="12" t="s">
         <v>2</v>
       </c>
       <c r="L79" s="5"/>
@@ -1976,8 +2286,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB076EE8-D0D3-4954-9948-E4CD27EFD4B6}">
   <dimension ref="A3:U242"/>
   <sheetViews>
-    <sheetView topLeftCell="A260" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="Z278" sqref="Z278"/>
+    <sheetView topLeftCell="A194" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="AA220" sqref="AA219:AA220"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18"/>
@@ -3047,7 +3357,7 @@
     </row>
     <row r="213" spans="1:20">
       <c r="A213" s="4"/>
-      <c r="C213" s="4" t="s">
+      <c r="C213" s="12" t="s">
         <v>30</v>
       </c>
       <c r="E213" s="5"/>
@@ -3205,8 +3515,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83097DD9-40C9-43A8-A2E7-318977E59DA9}">
   <dimension ref="A3:T118"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="AE21" sqref="AE21"/>
+    <sheetView topLeftCell="A79" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="Q86" sqref="Q86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18"/>
@@ -3245,647 +3555,124 @@
     </row>
     <row r="40" spans="1:20">
       <c r="A40" s="4"/>
-      <c r="B40" s="11"/>
-      <c r="C40" s="11"/>
-      <c r="D40" s="11"/>
-      <c r="E40" s="11"/>
-      <c r="F40" s="11"/>
-      <c r="G40" s="11"/>
-      <c r="H40" s="11"/>
-      <c r="I40" s="11"/>
-      <c r="J40" s="11"/>
-      <c r="K40" s="11"/>
-      <c r="L40" s="11"/>
-      <c r="M40" s="11"/>
-      <c r="N40" s="11"/>
-      <c r="O40" s="11"/>
-      <c r="P40" s="11"/>
-      <c r="Q40" s="11"/>
-      <c r="R40" s="11"/>
-      <c r="S40" s="11"/>
       <c r="T40" s="5"/>
     </row>
     <row r="41" spans="1:20">
       <c r="A41" s="4"/>
-      <c r="B41" s="11"/>
-      <c r="C41" s="11"/>
-      <c r="D41" s="11"/>
-      <c r="E41" s="11"/>
-      <c r="F41" s="11"/>
-      <c r="G41" s="11"/>
-      <c r="H41" s="11"/>
-      <c r="I41" s="11"/>
-      <c r="J41" s="11"/>
-      <c r="K41" s="11"/>
-      <c r="L41" s="11"/>
-      <c r="M41" s="11"/>
-      <c r="N41" s="11"/>
-      <c r="O41" s="11"/>
-      <c r="P41" s="11"/>
-      <c r="Q41" s="11"/>
-      <c r="R41" s="11"/>
-      <c r="S41" s="11"/>
       <c r="T41" s="5"/>
     </row>
     <row r="42" spans="1:20">
       <c r="A42" s="4"/>
-      <c r="B42" s="11"/>
-      <c r="C42" s="11"/>
-      <c r="D42" s="11"/>
-      <c r="E42" s="11"/>
-      <c r="F42" s="11"/>
-      <c r="G42" s="11"/>
-      <c r="H42" s="11"/>
-      <c r="I42" s="11"/>
-      <c r="J42" s="11"/>
-      <c r="K42" s="11"/>
-      <c r="L42" s="11"/>
-      <c r="M42" s="11"/>
-      <c r="N42" s="11"/>
-      <c r="O42" s="11"/>
-      <c r="P42" s="11"/>
-      <c r="Q42" s="11"/>
-      <c r="R42" s="11"/>
-      <c r="S42" s="11"/>
       <c r="T42" s="5"/>
     </row>
     <row r="43" spans="1:20">
       <c r="A43" s="4"/>
-      <c r="B43" s="11"/>
-      <c r="C43" s="11"/>
-      <c r="D43" s="11"/>
-      <c r="E43" s="11"/>
-      <c r="F43" s="11"/>
-      <c r="G43" s="11"/>
-      <c r="H43" s="11"/>
-      <c r="I43" s="11"/>
-      <c r="J43" s="11"/>
-      <c r="K43" s="11"/>
-      <c r="L43" s="11"/>
-      <c r="M43" s="11"/>
-      <c r="N43" s="11"/>
-      <c r="O43" s="11"/>
-      <c r="P43" s="11"/>
-      <c r="Q43" s="11"/>
-      <c r="R43" s="11"/>
-      <c r="S43" s="11"/>
       <c r="T43" s="5"/>
     </row>
     <row r="44" spans="1:20">
       <c r="A44" s="4"/>
-      <c r="B44" s="11"/>
-      <c r="C44" s="11"/>
-      <c r="D44" s="11"/>
-      <c r="E44" s="11"/>
-      <c r="F44" s="11"/>
-      <c r="G44" s="11"/>
-      <c r="H44" s="11"/>
-      <c r="I44" s="11"/>
-      <c r="J44" s="11"/>
-      <c r="K44" s="11"/>
-      <c r="L44" s="11"/>
-      <c r="M44" s="11"/>
-      <c r="N44" s="11"/>
-      <c r="O44" s="11"/>
-      <c r="P44" s="11"/>
-      <c r="Q44" s="11"/>
-      <c r="R44" s="11"/>
-      <c r="S44" s="11"/>
       <c r="T44" s="5"/>
     </row>
     <row r="45" spans="1:20">
       <c r="A45" s="4"/>
-      <c r="B45" s="11"/>
-      <c r="C45" s="11"/>
-      <c r="D45" s="11"/>
-      <c r="E45" s="11"/>
-      <c r="F45" s="11"/>
-      <c r="G45" s="11"/>
-      <c r="H45" s="11"/>
-      <c r="I45" s="11"/>
-      <c r="J45" s="11"/>
-      <c r="K45" s="11"/>
-      <c r="L45" s="11"/>
-      <c r="M45" s="11"/>
-      <c r="N45" s="11"/>
-      <c r="O45" s="11"/>
-      <c r="P45" s="11"/>
-      <c r="Q45" s="11"/>
-      <c r="R45" s="11"/>
-      <c r="S45" s="11"/>
       <c r="T45" s="5"/>
     </row>
     <row r="46" spans="1:20">
       <c r="A46" s="4"/>
-      <c r="B46" s="11"/>
-      <c r="C46" s="11"/>
-      <c r="D46" s="11"/>
-      <c r="E46" s="11"/>
-      <c r="F46" s="11"/>
-      <c r="G46" s="11"/>
-      <c r="H46" s="11"/>
-      <c r="I46" s="11"/>
-      <c r="J46" s="11"/>
-      <c r="K46" s="11"/>
-      <c r="L46" s="11"/>
-      <c r="M46" s="11"/>
-      <c r="N46" s="11"/>
-      <c r="O46" s="11"/>
-      <c r="P46" s="11"/>
-      <c r="Q46" s="11"/>
-      <c r="R46" s="11"/>
-      <c r="S46" s="11"/>
       <c r="T46" s="5"/>
     </row>
     <row r="47" spans="1:20">
       <c r="A47" s="4"/>
-      <c r="B47" s="11"/>
-      <c r="C47" s="11"/>
-      <c r="D47" s="11"/>
-      <c r="E47" s="11"/>
-      <c r="F47" s="11"/>
-      <c r="G47" s="11"/>
-      <c r="H47" s="11"/>
-      <c r="I47" s="11"/>
-      <c r="J47" s="11"/>
-      <c r="K47" s="11"/>
-      <c r="L47" s="11"/>
-      <c r="M47" s="11"/>
-      <c r="N47" s="11"/>
-      <c r="O47" s="11"/>
-      <c r="P47" s="11"/>
-      <c r="Q47" s="11"/>
-      <c r="R47" s="11"/>
-      <c r="S47" s="11"/>
       <c r="T47" s="5"/>
     </row>
     <row r="48" spans="1:20">
       <c r="A48" s="4"/>
-      <c r="B48" s="11"/>
-      <c r="C48" s="11"/>
-      <c r="D48" s="11"/>
-      <c r="E48" s="11"/>
-      <c r="F48" s="11"/>
-      <c r="G48" s="11"/>
-      <c r="H48" s="11"/>
-      <c r="I48" s="11"/>
-      <c r="J48" s="11"/>
-      <c r="K48" s="11"/>
-      <c r="L48" s="11"/>
-      <c r="M48" s="11"/>
-      <c r="N48" s="11"/>
-      <c r="O48" s="11"/>
-      <c r="P48" s="11"/>
-      <c r="Q48" s="11"/>
-      <c r="R48" s="11"/>
-      <c r="S48" s="11"/>
       <c r="T48" s="5"/>
     </row>
     <row r="49" spans="1:20">
       <c r="A49" s="4"/>
-      <c r="B49" s="11"/>
-      <c r="C49" s="11"/>
-      <c r="D49" s="11"/>
-      <c r="E49" s="11"/>
-      <c r="F49" s="11"/>
-      <c r="G49" s="11"/>
-      <c r="H49" s="11"/>
-      <c r="I49" s="11"/>
-      <c r="J49" s="11"/>
-      <c r="K49" s="11"/>
-      <c r="L49" s="11"/>
-      <c r="M49" s="11"/>
-      <c r="N49" s="11"/>
-      <c r="O49" s="11"/>
-      <c r="P49" s="11"/>
-      <c r="Q49" s="11"/>
-      <c r="R49" s="11"/>
-      <c r="S49" s="11"/>
       <c r="T49" s="5"/>
     </row>
     <row r="50" spans="1:20">
       <c r="A50" s="4"/>
-      <c r="B50" s="11"/>
-      <c r="C50" s="11"/>
-      <c r="D50" s="11"/>
-      <c r="E50" s="11"/>
-      <c r="F50" s="11"/>
-      <c r="G50" s="11"/>
-      <c r="H50" s="11"/>
-      <c r="I50" s="11"/>
-      <c r="J50" s="11"/>
-      <c r="K50" s="11"/>
-      <c r="L50" s="11"/>
-      <c r="M50" s="11"/>
-      <c r="N50" s="11"/>
-      <c r="O50" s="11"/>
-      <c r="P50" s="11"/>
-      <c r="Q50" s="11"/>
-      <c r="R50" s="11"/>
-      <c r="S50" s="11"/>
       <c r="T50" s="5"/>
     </row>
     <row r="51" spans="1:20">
       <c r="A51" s="4"/>
-      <c r="B51" s="11"/>
-      <c r="C51" s="11"/>
-      <c r="D51" s="11"/>
-      <c r="E51" s="11"/>
-      <c r="F51" s="11"/>
-      <c r="G51" s="11"/>
-      <c r="H51" s="11"/>
-      <c r="I51" s="11"/>
-      <c r="J51" s="11"/>
-      <c r="K51" s="11"/>
-      <c r="L51" s="11"/>
-      <c r="M51" s="11"/>
-      <c r="N51" s="11"/>
-      <c r="O51" s="11"/>
-      <c r="P51" s="11"/>
-      <c r="Q51" s="11"/>
-      <c r="R51" s="11"/>
-      <c r="S51" s="11"/>
       <c r="T51" s="5"/>
     </row>
     <row r="52" spans="1:20">
       <c r="A52" s="4"/>
-      <c r="B52" s="11"/>
-      <c r="C52" s="11"/>
-      <c r="D52" s="11"/>
-      <c r="E52" s="11"/>
-      <c r="F52" s="11"/>
-      <c r="G52" s="11"/>
-      <c r="H52" s="11"/>
-      <c r="I52" s="11"/>
-      <c r="J52" s="11"/>
-      <c r="K52" s="11"/>
-      <c r="L52" s="11"/>
-      <c r="M52" s="11"/>
-      <c r="N52" s="11"/>
-      <c r="O52" s="11"/>
-      <c r="P52" s="11"/>
-      <c r="Q52" s="11"/>
-      <c r="R52" s="11"/>
-      <c r="S52" s="11"/>
       <c r="T52" s="5"/>
     </row>
     <row r="53" spans="1:20">
       <c r="A53" s="4"/>
-      <c r="B53" s="11"/>
-      <c r="C53" s="11"/>
-      <c r="D53" s="11"/>
-      <c r="E53" s="11"/>
-      <c r="F53" s="11"/>
-      <c r="G53" s="11"/>
-      <c r="H53" s="11"/>
-      <c r="I53" s="11"/>
-      <c r="J53" s="11"/>
-      <c r="K53" s="11"/>
-      <c r="L53" s="11"/>
-      <c r="M53" s="11"/>
-      <c r="N53" s="11"/>
-      <c r="O53" s="11"/>
-      <c r="P53" s="11"/>
-      <c r="Q53" s="11"/>
-      <c r="R53" s="11"/>
-      <c r="S53" s="11"/>
       <c r="T53" s="5"/>
     </row>
     <row r="54" spans="1:20">
       <c r="A54" s="4"/>
-      <c r="B54" s="11"/>
-      <c r="C54" s="11"/>
-      <c r="D54" s="11"/>
-      <c r="E54" s="11"/>
-      <c r="F54" s="11"/>
-      <c r="G54" s="11"/>
-      <c r="H54" s="11"/>
-      <c r="I54" s="11"/>
-      <c r="J54" s="11"/>
-      <c r="K54" s="11"/>
-      <c r="L54" s="11"/>
-      <c r="M54" s="11"/>
-      <c r="N54" s="11"/>
-      <c r="O54" s="11"/>
-      <c r="P54" s="11"/>
-      <c r="Q54" s="11"/>
-      <c r="R54" s="11"/>
-      <c r="S54" s="11"/>
       <c r="T54" s="5"/>
     </row>
     <row r="55" spans="1:20">
       <c r="A55" s="4"/>
-      <c r="B55" s="11"/>
-      <c r="C55" s="11"/>
-      <c r="D55" s="11"/>
-      <c r="E55" s="11"/>
-      <c r="F55" s="11"/>
-      <c r="G55" s="11"/>
-      <c r="H55" s="11"/>
-      <c r="I55" s="11"/>
-      <c r="J55" s="11"/>
-      <c r="K55" s="11"/>
-      <c r="L55" s="11"/>
-      <c r="M55" s="11"/>
-      <c r="N55" s="11"/>
-      <c r="O55" s="11"/>
-      <c r="P55" s="11"/>
-      <c r="Q55" s="11"/>
-      <c r="R55" s="11"/>
-      <c r="S55" s="11"/>
       <c r="T55" s="5"/>
     </row>
     <row r="56" spans="1:20">
       <c r="A56" s="4"/>
-      <c r="B56" s="11"/>
-      <c r="C56" s="11"/>
-      <c r="D56" s="11"/>
-      <c r="E56" s="11"/>
-      <c r="F56" s="11"/>
-      <c r="G56" s="11"/>
-      <c r="H56" s="11"/>
-      <c r="I56" s="11"/>
-      <c r="J56" s="11"/>
-      <c r="K56" s="11"/>
-      <c r="L56" s="11"/>
-      <c r="M56" s="11"/>
-      <c r="N56" s="11"/>
-      <c r="O56" s="11"/>
-      <c r="P56" s="11"/>
-      <c r="Q56" s="11"/>
-      <c r="R56" s="11"/>
-      <c r="S56" s="11"/>
       <c r="T56" s="5"/>
     </row>
     <row r="57" spans="1:20">
       <c r="A57" s="4"/>
-      <c r="B57" s="11"/>
-      <c r="C57" s="11"/>
-      <c r="D57" s="11"/>
-      <c r="E57" s="11"/>
-      <c r="F57" s="11"/>
-      <c r="G57" s="11"/>
-      <c r="H57" s="11"/>
-      <c r="I57" s="11"/>
-      <c r="J57" s="11"/>
-      <c r="K57" s="11"/>
-      <c r="L57" s="11"/>
-      <c r="M57" s="11"/>
-      <c r="N57" s="11"/>
-      <c r="O57" s="11"/>
-      <c r="P57" s="11"/>
-      <c r="Q57" s="11"/>
-      <c r="R57" s="11"/>
-      <c r="S57" s="11"/>
       <c r="T57" s="5"/>
     </row>
     <row r="58" spans="1:20">
       <c r="A58" s="4"/>
-      <c r="B58" s="11"/>
-      <c r="C58" s="11"/>
-      <c r="D58" s="11"/>
-      <c r="E58" s="11"/>
-      <c r="F58" s="11"/>
-      <c r="G58" s="11"/>
-      <c r="H58" s="11"/>
-      <c r="I58" s="11"/>
-      <c r="J58" s="11"/>
-      <c r="K58" s="11"/>
-      <c r="L58" s="11"/>
-      <c r="M58" s="11"/>
-      <c r="N58" s="11"/>
-      <c r="O58" s="11"/>
-      <c r="P58" s="11"/>
-      <c r="Q58" s="11"/>
-      <c r="R58" s="11"/>
-      <c r="S58" s="11"/>
       <c r="T58" s="5"/>
     </row>
     <row r="59" spans="1:20">
       <c r="A59" s="4"/>
-      <c r="B59" s="11"/>
-      <c r="C59" s="11"/>
-      <c r="D59" s="11"/>
-      <c r="E59" s="11"/>
-      <c r="F59" s="11"/>
-      <c r="G59" s="11"/>
-      <c r="H59" s="11"/>
-      <c r="I59" s="11"/>
-      <c r="J59" s="11"/>
-      <c r="K59" s="11"/>
-      <c r="L59" s="11"/>
-      <c r="M59" s="11"/>
-      <c r="N59" s="11"/>
-      <c r="O59" s="11"/>
-      <c r="P59" s="11"/>
-      <c r="Q59" s="11"/>
-      <c r="R59" s="11"/>
-      <c r="S59" s="11"/>
       <c r="T59" s="5"/>
     </row>
     <row r="60" spans="1:20">
       <c r="A60" s="4"/>
-      <c r="B60" s="11"/>
-      <c r="C60" s="11"/>
-      <c r="D60" s="11"/>
-      <c r="E60" s="11"/>
-      <c r="F60" s="11"/>
-      <c r="G60" s="11"/>
-      <c r="H60" s="11"/>
-      <c r="I60" s="11"/>
-      <c r="J60" s="11"/>
-      <c r="K60" s="11"/>
-      <c r="L60" s="11"/>
-      <c r="M60" s="11"/>
-      <c r="N60" s="11"/>
-      <c r="O60" s="11"/>
-      <c r="P60" s="11"/>
-      <c r="Q60" s="11"/>
-      <c r="R60" s="11"/>
-      <c r="S60" s="11"/>
       <c r="T60" s="5"/>
     </row>
     <row r="61" spans="1:20">
       <c r="A61" s="4"/>
-      <c r="B61" s="11"/>
-      <c r="C61" s="11"/>
-      <c r="D61" s="11"/>
-      <c r="E61" s="11"/>
-      <c r="F61" s="11"/>
-      <c r="G61" s="11"/>
-      <c r="H61" s="11"/>
-      <c r="I61" s="11"/>
-      <c r="J61" s="11"/>
-      <c r="K61" s="11"/>
-      <c r="L61" s="11"/>
-      <c r="M61" s="11"/>
-      <c r="N61" s="11"/>
-      <c r="O61" s="11"/>
-      <c r="P61" s="11"/>
-      <c r="Q61" s="11"/>
-      <c r="R61" s="11"/>
-      <c r="S61" s="11"/>
       <c r="T61" s="5"/>
     </row>
     <row r="62" spans="1:20">
       <c r="A62" s="4"/>
-      <c r="B62" s="11"/>
-      <c r="C62" s="11"/>
-      <c r="D62" s="11"/>
-      <c r="E62" s="11"/>
-      <c r="F62" s="11"/>
-      <c r="G62" s="11"/>
-      <c r="H62" s="11"/>
-      <c r="I62" s="11"/>
-      <c r="J62" s="11"/>
-      <c r="K62" s="11"/>
-      <c r="L62" s="11"/>
-      <c r="M62" s="11"/>
-      <c r="N62" s="11"/>
-      <c r="O62" s="11"/>
-      <c r="P62" s="11"/>
-      <c r="Q62" s="11"/>
-      <c r="R62" s="11"/>
-      <c r="S62" s="11"/>
       <c r="T62" s="5"/>
     </row>
     <row r="63" spans="1:20">
       <c r="A63" s="4"/>
-      <c r="B63" s="11"/>
-      <c r="C63" s="11"/>
-      <c r="D63" s="11"/>
-      <c r="E63" s="11"/>
-      <c r="F63" s="11"/>
-      <c r="G63" s="11"/>
-      <c r="H63" s="11"/>
-      <c r="I63" s="11"/>
-      <c r="J63" s="11"/>
-      <c r="K63" s="11"/>
-      <c r="L63" s="11"/>
-      <c r="M63" s="11"/>
-      <c r="N63" s="11"/>
-      <c r="O63" s="11"/>
-      <c r="P63" s="11"/>
-      <c r="Q63" s="11"/>
-      <c r="R63" s="11"/>
-      <c r="S63" s="11"/>
       <c r="T63" s="5"/>
     </row>
     <row r="64" spans="1:20">
       <c r="A64" s="4"/>
-      <c r="B64" s="11"/>
-      <c r="C64" s="11"/>
-      <c r="D64" s="11"/>
-      <c r="E64" s="11"/>
-      <c r="F64" s="11"/>
-      <c r="G64" s="11"/>
-      <c r="H64" s="11"/>
-      <c r="I64" s="11"/>
-      <c r="J64" s="11"/>
-      <c r="K64" s="11"/>
-      <c r="L64" s="11"/>
-      <c r="M64" s="11"/>
-      <c r="N64" s="11"/>
-      <c r="O64" s="11"/>
-      <c r="P64" s="11"/>
-      <c r="Q64" s="11"/>
-      <c r="R64" s="11"/>
-      <c r="S64" s="11"/>
       <c r="T64" s="5"/>
     </row>
     <row r="65" spans="1:20">
       <c r="A65" s="4"/>
-      <c r="B65" s="11"/>
-      <c r="C65" s="11"/>
-      <c r="D65" s="11"/>
-      <c r="E65" s="11"/>
-      <c r="F65" s="11"/>
-      <c r="G65" s="11"/>
-      <c r="H65" s="11"/>
-      <c r="I65" s="11"/>
-      <c r="J65" s="11"/>
-      <c r="K65" s="11"/>
-      <c r="L65" s="11"/>
-      <c r="M65" s="11"/>
-      <c r="N65" s="11"/>
-      <c r="O65" s="11"/>
-      <c r="P65" s="11"/>
-      <c r="Q65" s="11"/>
-      <c r="R65" s="11"/>
-      <c r="S65" s="11"/>
       <c r="T65" s="5"/>
     </row>
     <row r="66" spans="1:20">
       <c r="A66" s="4"/>
-      <c r="B66" s="11"/>
-      <c r="C66" s="11"/>
-      <c r="D66" s="11"/>
-      <c r="E66" s="11"/>
-      <c r="F66" s="11"/>
-      <c r="G66" s="11"/>
-      <c r="H66" s="11"/>
-      <c r="I66" s="11"/>
-      <c r="J66" s="11"/>
-      <c r="K66" s="11"/>
-      <c r="L66" s="11"/>
-      <c r="M66" s="11"/>
-      <c r="N66" s="11"/>
-      <c r="O66" s="11"/>
-      <c r="P66" s="11"/>
-      <c r="Q66" s="11"/>
-      <c r="R66" s="11"/>
-      <c r="S66" s="11"/>
       <c r="T66" s="5"/>
     </row>
     <row r="67" spans="1:20">
       <c r="A67" s="4"/>
-      <c r="B67" s="11"/>
-      <c r="C67" s="11"/>
-      <c r="D67" s="11"/>
-      <c r="E67" s="11"/>
-      <c r="F67" s="11"/>
-      <c r="G67" s="11"/>
-      <c r="H67" s="11"/>
-      <c r="I67" s="11"/>
-      <c r="J67" s="11"/>
-      <c r="K67" s="11"/>
-      <c r="L67" s="11"/>
-      <c r="M67" s="11"/>
-      <c r="N67" s="11"/>
-      <c r="O67" s="11"/>
-      <c r="P67" s="11"/>
-      <c r="Q67" s="11"/>
-      <c r="R67" s="11"/>
-      <c r="S67" s="11"/>
       <c r="T67" s="5"/>
     </row>
     <row r="68" spans="1:20">
       <c r="A68" s="4"/>
-      <c r="B68" s="11"/>
-      <c r="C68" s="11"/>
-      <c r="D68" s="11"/>
-      <c r="E68" s="11"/>
-      <c r="F68" s="11"/>
-      <c r="G68" s="11"/>
-      <c r="H68" s="11"/>
-      <c r="I68" s="11"/>
-      <c r="J68" s="11"/>
-      <c r="K68" s="11"/>
-      <c r="L68" s="11"/>
-      <c r="M68" s="11"/>
-      <c r="N68" s="11"/>
-      <c r="O68" s="11"/>
-      <c r="P68" s="11"/>
-      <c r="Q68" s="11"/>
-      <c r="R68" s="11"/>
-      <c r="S68" s="11"/>
       <c r="T68" s="5"/>
     </row>
     <row r="69" spans="1:20">
       <c r="A69" s="4"/>
-      <c r="B69" s="11"/>
       <c r="C69" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D69" s="2"/>
       <c r="E69" s="2"/>
@@ -3895,239 +3682,70 @@
       <c r="I69" s="2"/>
       <c r="J69" s="2"/>
       <c r="K69" s="3"/>
-      <c r="L69" s="11"/>
-      <c r="M69" s="11"/>
-      <c r="N69" s="11"/>
-      <c r="O69" s="11"/>
-      <c r="P69" s="11"/>
-      <c r="Q69" s="11"/>
-      <c r="R69" s="11"/>
-      <c r="S69" s="11"/>
       <c r="T69" s="5"/>
     </row>
     <row r="70" spans="1:20">
       <c r="A70" s="4"/>
-      <c r="B70" s="11"/>
       <c r="C70" s="4"/>
-      <c r="D70" s="11"/>
-      <c r="E70" s="11"/>
-      <c r="F70" s="11"/>
-      <c r="G70" s="11"/>
-      <c r="H70" s="11"/>
-      <c r="I70" s="11"/>
-      <c r="J70" s="11"/>
       <c r="K70" s="5"/>
-      <c r="L70" s="11"/>
-      <c r="M70" s="11"/>
-      <c r="N70" s="11"/>
-      <c r="O70" s="11"/>
-      <c r="P70" s="11"/>
-      <c r="Q70" s="11"/>
-      <c r="R70" s="11"/>
-      <c r="S70" s="11"/>
       <c r="T70" s="5"/>
     </row>
     <row r="71" spans="1:20">
       <c r="A71" s="4"/>
-      <c r="B71" s="11"/>
       <c r="C71" s="4"/>
-      <c r="D71" s="11"/>
-      <c r="E71" s="11"/>
-      <c r="F71" s="11"/>
-      <c r="G71" s="11"/>
-      <c r="H71" s="11"/>
-      <c r="I71" s="11"/>
-      <c r="J71" s="11"/>
       <c r="K71" s="5"/>
-      <c r="L71" s="11"/>
-      <c r="M71" s="11"/>
-      <c r="N71" s="11"/>
-      <c r="O71" s="11"/>
-      <c r="P71" s="11"/>
-      <c r="Q71" s="11"/>
-      <c r="R71" s="11"/>
-      <c r="S71" s="11"/>
       <c r="T71" s="5"/>
     </row>
     <row r="72" spans="1:20">
       <c r="A72" s="4"/>
-      <c r="B72" s="11"/>
       <c r="C72" s="4"/>
-      <c r="D72" s="11"/>
-      <c r="E72" s="11"/>
-      <c r="F72" s="11"/>
-      <c r="G72" s="11"/>
-      <c r="H72" s="11"/>
-      <c r="I72" s="11"/>
-      <c r="J72" s="11"/>
       <c r="K72" s="5"/>
-      <c r="L72" s="11"/>
-      <c r="M72" s="11"/>
-      <c r="N72" s="11"/>
-      <c r="O72" s="11"/>
-      <c r="P72" s="11"/>
-      <c r="Q72" s="11"/>
-      <c r="R72" s="11"/>
-      <c r="S72" s="11"/>
       <c r="T72" s="5"/>
     </row>
     <row r="73" spans="1:20">
       <c r="A73" s="4"/>
-      <c r="B73" s="11"/>
       <c r="C73" s="4"/>
-      <c r="D73" s="11"/>
-      <c r="E73" s="11"/>
-      <c r="F73" s="11"/>
-      <c r="G73" s="11"/>
-      <c r="H73" s="11"/>
-      <c r="I73" s="11"/>
-      <c r="J73" s="11"/>
       <c r="K73" s="5"/>
-      <c r="L73" s="11"/>
-      <c r="M73" s="11"/>
-      <c r="N73" s="11"/>
-      <c r="O73" s="11"/>
-      <c r="P73" s="11"/>
-      <c r="Q73" s="11"/>
-      <c r="R73" s="11"/>
-      <c r="S73" s="11"/>
       <c r="T73" s="5"/>
     </row>
     <row r="74" spans="1:20">
       <c r="A74" s="4"/>
-      <c r="B74" s="11"/>
       <c r="C74" s="4"/>
-      <c r="D74" s="11"/>
-      <c r="E74" s="11"/>
-      <c r="F74" s="11"/>
-      <c r="G74" s="11"/>
-      <c r="H74" s="11"/>
-      <c r="I74" s="11"/>
-      <c r="J74" s="11"/>
       <c r="K74" s="5"/>
-      <c r="L74" s="11"/>
-      <c r="M74" s="11"/>
-      <c r="N74" s="11"/>
-      <c r="O74" s="11"/>
-      <c r="P74" s="11"/>
-      <c r="Q74" s="11"/>
-      <c r="R74" s="11"/>
-      <c r="S74" s="11"/>
       <c r="T74" s="5"/>
     </row>
     <row r="75" spans="1:20">
       <c r="A75" s="4"/>
-      <c r="B75" s="11"/>
       <c r="C75" s="4"/>
-      <c r="D75" s="11"/>
-      <c r="E75" s="11"/>
-      <c r="F75" s="11"/>
-      <c r="G75" s="11"/>
-      <c r="H75" s="11"/>
-      <c r="I75" s="11"/>
-      <c r="J75" s="11"/>
       <c r="K75" s="5"/>
-      <c r="L75" s="11"/>
-      <c r="M75" s="11"/>
-      <c r="N75" s="11"/>
-      <c r="O75" s="11"/>
-      <c r="P75" s="11"/>
-      <c r="Q75" s="11"/>
-      <c r="R75" s="11"/>
-      <c r="S75" s="11"/>
       <c r="T75" s="5"/>
     </row>
     <row r="76" spans="1:20">
       <c r="A76" s="4"/>
-      <c r="B76" s="11"/>
       <c r="C76" s="4"/>
-      <c r="D76" s="11"/>
-      <c r="E76" s="11"/>
-      <c r="F76" s="11"/>
-      <c r="G76" s="11"/>
-      <c r="H76" s="11"/>
-      <c r="I76" s="11"/>
-      <c r="J76" s="11"/>
       <c r="K76" s="5"/>
-      <c r="L76" s="11"/>
-      <c r="M76" s="11"/>
-      <c r="N76" s="11"/>
-      <c r="O76" s="11"/>
-      <c r="P76" s="11"/>
-      <c r="Q76" s="11"/>
-      <c r="R76" s="11"/>
-      <c r="S76" s="11"/>
       <c r="T76" s="5"/>
     </row>
     <row r="77" spans="1:20">
       <c r="A77" s="4"/>
-      <c r="B77" s="11"/>
       <c r="C77" s="4"/>
-      <c r="D77" s="11"/>
-      <c r="E77" s="11"/>
-      <c r="F77" s="11"/>
-      <c r="G77" s="11"/>
-      <c r="H77" s="11"/>
-      <c r="I77" s="11"/>
-      <c r="J77" s="11"/>
       <c r="K77" s="5"/>
-      <c r="L77" s="11"/>
-      <c r="M77" s="11"/>
-      <c r="N77" s="11"/>
-      <c r="O77" s="11"/>
-      <c r="P77" s="11"/>
-      <c r="Q77" s="11"/>
-      <c r="R77" s="11"/>
-      <c r="S77" s="11"/>
       <c r="T77" s="5"/>
     </row>
     <row r="78" spans="1:20">
       <c r="A78" s="4"/>
-      <c r="B78" s="11"/>
       <c r="C78" s="4"/>
-      <c r="D78" s="11"/>
-      <c r="E78" s="11"/>
-      <c r="F78" s="11"/>
-      <c r="G78" s="11"/>
-      <c r="H78" s="11"/>
-      <c r="I78" s="11"/>
-      <c r="J78" s="11"/>
       <c r="K78" s="5"/>
-      <c r="L78" s="11"/>
-      <c r="M78" s="11"/>
-      <c r="N78" s="11"/>
-      <c r="O78" s="11"/>
-      <c r="P78" s="11"/>
-      <c r="Q78" s="11"/>
-      <c r="R78" s="11"/>
-      <c r="S78" s="11"/>
       <c r="T78" s="5"/>
     </row>
     <row r="79" spans="1:20">
       <c r="A79" s="4"/>
-      <c r="B79" s="11"/>
       <c r="C79" s="4"/>
-      <c r="D79" s="11"/>
-      <c r="E79" s="11"/>
-      <c r="F79" s="11"/>
-      <c r="G79" s="11"/>
-      <c r="H79" s="11"/>
-      <c r="I79" s="11"/>
-      <c r="J79" s="11"/>
       <c r="K79" s="5"/>
-      <c r="L79" s="11"/>
-      <c r="M79" s="11"/>
-      <c r="N79" s="11"/>
-      <c r="O79" s="11"/>
-      <c r="P79" s="11"/>
-      <c r="Q79" s="11"/>
-      <c r="R79" s="11"/>
-      <c r="S79" s="11"/>
       <c r="T79" s="5"/>
     </row>
     <row r="80" spans="1:20">
       <c r="A80" s="4"/>
-      <c r="B80" s="11"/>
       <c r="C80" s="6"/>
       <c r="D80" s="7"/>
       <c r="E80" s="7"/>
@@ -4137,846 +3755,200 @@
       <c r="I80" s="7"/>
       <c r="J80" s="7"/>
       <c r="K80" s="8"/>
-      <c r="L80" s="11"/>
-      <c r="M80" s="11"/>
-      <c r="N80" s="11"/>
-      <c r="O80" s="11"/>
-      <c r="P80" s="11"/>
-      <c r="Q80" s="11"/>
-      <c r="R80" s="11"/>
-      <c r="S80" s="11"/>
       <c r="T80" s="5"/>
     </row>
     <row r="81" spans="1:20">
       <c r="A81" s="4"/>
-      <c r="B81" s="11"/>
-      <c r="C81" s="11"/>
-      <c r="D81" s="11"/>
-      <c r="E81" s="11"/>
-      <c r="F81" s="11"/>
-      <c r="G81" s="11"/>
-      <c r="H81" s="11"/>
-      <c r="I81" s="11"/>
-      <c r="J81" s="11"/>
-      <c r="K81" s="11"/>
-      <c r="L81" s="11"/>
-      <c r="M81" s="11"/>
-      <c r="N81" s="11"/>
-      <c r="O81" s="11"/>
-      <c r="P81" s="11"/>
-      <c r="Q81" s="11"/>
-      <c r="R81" s="11"/>
-      <c r="S81" s="11"/>
       <c r="T81" s="5"/>
     </row>
     <row r="82" spans="1:20">
       <c r="A82" s="4"/>
-      <c r="B82" s="11"/>
-      <c r="C82" s="11"/>
-      <c r="D82" s="11"/>
-      <c r="E82" s="11"/>
-      <c r="F82" s="11"/>
-      <c r="G82" s="11"/>
-      <c r="H82" s="11"/>
-      <c r="I82" s="11"/>
-      <c r="J82" s="11"/>
-      <c r="K82" s="11"/>
-      <c r="L82" s="11"/>
-      <c r="M82" s="11"/>
-      <c r="N82" s="11"/>
-      <c r="O82" s="11"/>
-      <c r="P82" s="11"/>
-      <c r="Q82" s="11"/>
-      <c r="R82" s="11"/>
-      <c r="S82" s="11"/>
       <c r="T82" s="5"/>
     </row>
     <row r="83" spans="1:20">
       <c r="A83" s="4"/>
-      <c r="B83" s="11"/>
       <c r="C83" s="1" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="D83" s="2"/>
       <c r="E83" s="2"/>
       <c r="F83" s="2"/>
       <c r="G83" s="2"/>
       <c r="H83" s="3"/>
-      <c r="I83" s="11"/>
-      <c r="J83" s="11"/>
-      <c r="K83" s="11"/>
-      <c r="L83" s="11"/>
-      <c r="M83" s="11"/>
-      <c r="N83" s="11"/>
-      <c r="O83" s="11"/>
-      <c r="P83" s="11"/>
-      <c r="Q83" s="11"/>
-      <c r="R83" s="11"/>
-      <c r="S83" s="11"/>
       <c r="T83" s="5"/>
     </row>
     <row r="84" spans="1:20">
       <c r="A84" s="4"/>
-      <c r="B84" s="11"/>
-      <c r="C84" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="D84" s="11"/>
-      <c r="E84" s="11"/>
-      <c r="F84" s="11"/>
-      <c r="G84" s="11"/>
+      <c r="C84" s="12" t="s">
+        <v>34</v>
+      </c>
       <c r="H84" s="5"/>
-      <c r="I84" s="11"/>
-      <c r="J84" s="11"/>
-      <c r="K84" s="11"/>
-      <c r="L84" s="11"/>
-      <c r="M84" s="11"/>
-      <c r="N84" s="11"/>
-      <c r="O84" s="11"/>
-      <c r="P84" s="11"/>
-      <c r="Q84" s="11"/>
-      <c r="R84" s="11"/>
-      <c r="S84" s="11"/>
       <c r="T84" s="5"/>
     </row>
     <row r="85" spans="1:20">
       <c r="A85" s="4"/>
-      <c r="B85" s="11"/>
-      <c r="C85" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="D85" s="11"/>
-      <c r="E85" s="11"/>
-      <c r="F85" s="11"/>
-      <c r="G85" s="11"/>
+      <c r="C85" s="13" t="s">
+        <v>35</v>
+      </c>
       <c r="H85" s="5"/>
-      <c r="I85" s="11"/>
-      <c r="J85" s="11"/>
-      <c r="K85" s="11"/>
-      <c r="L85" s="11"/>
-      <c r="M85" s="11"/>
-      <c r="N85" s="11"/>
-      <c r="O85" s="11"/>
-      <c r="P85" s="11"/>
-      <c r="Q85" s="11"/>
-      <c r="R85" s="11"/>
-      <c r="S85" s="11"/>
       <c r="T85" s="5"/>
     </row>
     <row r="86" spans="1:20">
       <c r="A86" s="4"/>
-      <c r="B86" s="11"/>
-      <c r="C86" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="D86" s="11"/>
-      <c r="E86" s="11"/>
-      <c r="F86" s="11"/>
-      <c r="G86" s="11"/>
+      <c r="C86" s="13" t="s">
+        <v>36</v>
+      </c>
       <c r="H86" s="5"/>
-      <c r="I86" s="11"/>
-      <c r="J86" s="11"/>
-      <c r="K86" s="11"/>
-      <c r="L86" s="11"/>
-      <c r="M86" s="11"/>
-      <c r="N86" s="11"/>
-      <c r="O86" s="11"/>
-      <c r="P86" s="11"/>
-      <c r="Q86" s="11"/>
-      <c r="R86" s="11"/>
-      <c r="S86" s="11"/>
       <c r="T86" s="5"/>
     </row>
     <row r="87" spans="1:20">
       <c r="A87" s="4"/>
-      <c r="B87" s="11"/>
-      <c r="C87" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="D87" s="11"/>
-      <c r="E87" s="11"/>
-      <c r="F87" s="11"/>
-      <c r="G87" s="11"/>
+      <c r="C87" s="13" t="s">
+        <v>37</v>
+      </c>
       <c r="H87" s="5"/>
-      <c r="I87" s="11"/>
-      <c r="J87" s="11"/>
-      <c r="K87" s="11"/>
-      <c r="L87" s="11"/>
-      <c r="M87" s="11"/>
-      <c r="N87" s="11"/>
-      <c r="O87" s="11"/>
-      <c r="P87" s="11"/>
-      <c r="Q87" s="11"/>
-      <c r="R87" s="11"/>
-      <c r="S87" s="11"/>
       <c r="T87" s="5"/>
     </row>
     <row r="88" spans="1:20">
       <c r="A88" s="4"/>
-      <c r="B88" s="11"/>
-      <c r="C88" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="D88" s="11"/>
-      <c r="E88" s="11"/>
-      <c r="F88" s="11"/>
-      <c r="G88" s="11"/>
+      <c r="C88" s="13" t="s">
+        <v>38</v>
+      </c>
       <c r="H88" s="5"/>
-      <c r="I88" s="11"/>
-      <c r="J88" s="11"/>
-      <c r="K88" s="11"/>
-      <c r="L88" s="11"/>
-      <c r="M88" s="11"/>
-      <c r="N88" s="11"/>
-      <c r="O88" s="11"/>
-      <c r="P88" s="11"/>
-      <c r="Q88" s="11"/>
-      <c r="R88" s="11"/>
-      <c r="S88" s="11"/>
       <c r="T88" s="5"/>
     </row>
     <row r="89" spans="1:20">
       <c r="A89" s="4"/>
-      <c r="B89" s="11"/>
-      <c r="C89" s="4" t="s">
+      <c r="C89" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="D89" s="11"/>
-      <c r="E89" s="11"/>
-      <c r="F89" s="11"/>
-      <c r="G89" s="11"/>
       <c r="H89" s="5"/>
-      <c r="I89" s="11"/>
-      <c r="J89" s="11"/>
-      <c r="K89" s="11"/>
-      <c r="L89" s="11"/>
-      <c r="M89" s="11"/>
-      <c r="N89" s="11"/>
-      <c r="O89" s="11"/>
-      <c r="P89" s="11"/>
-      <c r="Q89" s="11"/>
-      <c r="R89" s="11"/>
-      <c r="S89" s="11"/>
       <c r="T89" s="5"/>
     </row>
     <row r="90" spans="1:20">
       <c r="A90" s="4"/>
-      <c r="B90" s="11"/>
-      <c r="C90" s="4" t="s">
+      <c r="C90" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="D90" s="11"/>
-      <c r="E90" s="11"/>
-      <c r="F90" s="11"/>
-      <c r="G90" s="11"/>
       <c r="H90" s="5"/>
-      <c r="I90" s="11"/>
-      <c r="J90" s="11"/>
-      <c r="K90" s="11"/>
-      <c r="L90" s="11"/>
-      <c r="M90" s="11"/>
-      <c r="N90" s="11"/>
-      <c r="O90" s="11"/>
-      <c r="P90" s="11"/>
-      <c r="Q90" s="11"/>
-      <c r="R90" s="11"/>
-      <c r="S90" s="11"/>
       <c r="T90" s="5"/>
     </row>
     <row r="91" spans="1:20">
       <c r="A91" s="4"/>
-      <c r="B91" s="11"/>
       <c r="C91" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D91" s="11"/>
-      <c r="E91" s="11"/>
-      <c r="F91" s="11"/>
-      <c r="G91" s="11"/>
       <c r="H91" s="5"/>
-      <c r="I91" s="11"/>
-      <c r="J91" s="11"/>
-      <c r="K91" s="11"/>
-      <c r="L91" s="11"/>
-      <c r="M91" s="11"/>
-      <c r="N91" s="11"/>
-      <c r="O91" s="11"/>
-      <c r="P91" s="11"/>
-      <c r="Q91" s="11"/>
-      <c r="R91" s="11"/>
-      <c r="S91" s="11"/>
       <c r="T91" s="5"/>
     </row>
     <row r="92" spans="1:20">
       <c r="A92" s="4"/>
-      <c r="B92" s="11"/>
       <c r="C92" s="6"/>
       <c r="D92" s="7"/>
       <c r="E92" s="7"/>
       <c r="F92" s="7"/>
       <c r="G92" s="7"/>
       <c r="H92" s="8"/>
-      <c r="I92" s="11"/>
-      <c r="J92" s="11"/>
-      <c r="K92" s="11"/>
-      <c r="L92" s="11"/>
-      <c r="M92" s="11"/>
-      <c r="N92" s="11"/>
-      <c r="O92" s="11"/>
-      <c r="P92" s="11"/>
-      <c r="Q92" s="11"/>
-      <c r="R92" s="11"/>
-      <c r="S92" s="11"/>
       <c r="T92" s="5"/>
     </row>
     <row r="93" spans="1:20">
       <c r="A93" s="4"/>
-      <c r="B93" s="11"/>
-      <c r="C93" s="11"/>
-      <c r="D93" s="11"/>
-      <c r="E93" s="11"/>
-      <c r="F93" s="11"/>
-      <c r="G93" s="11"/>
-      <c r="H93" s="11"/>
-      <c r="I93" s="11"/>
-      <c r="J93" s="11"/>
-      <c r="K93" s="11"/>
-      <c r="L93" s="11"/>
-      <c r="M93" s="11"/>
-      <c r="N93" s="11"/>
-      <c r="O93" s="11"/>
-      <c r="P93" s="11"/>
-      <c r="Q93" s="11"/>
-      <c r="R93" s="11"/>
-      <c r="S93" s="11"/>
       <c r="T93" s="5"/>
     </row>
     <row r="94" spans="1:20">
       <c r="A94" s="4"/>
-      <c r="B94" s="11"/>
-      <c r="C94" s="11"/>
-      <c r="D94" s="11"/>
-      <c r="E94" s="11"/>
-      <c r="F94" s="11"/>
-      <c r="G94" s="11"/>
-      <c r="H94" s="11"/>
-      <c r="I94" s="11"/>
-      <c r="J94" s="11"/>
-      <c r="K94" s="11"/>
-      <c r="L94" s="11"/>
-      <c r="M94" s="11"/>
-      <c r="N94" s="11"/>
-      <c r="O94" s="11"/>
-      <c r="P94" s="11"/>
-      <c r="Q94" s="11"/>
-      <c r="R94" s="11"/>
-      <c r="S94" s="11"/>
       <c r="T94" s="5"/>
     </row>
     <row r="95" spans="1:20">
       <c r="A95" s="4"/>
-      <c r="B95" s="11"/>
-      <c r="C95" s="11"/>
-      <c r="D95" s="11"/>
-      <c r="E95" s="11"/>
-      <c r="F95" s="11"/>
-      <c r="G95" s="11"/>
-      <c r="H95" s="11"/>
-      <c r="I95" s="11"/>
-      <c r="J95" s="11"/>
-      <c r="K95" s="11"/>
-      <c r="L95" s="11"/>
-      <c r="M95" s="11"/>
-      <c r="N95" s="11"/>
-      <c r="O95" s="11"/>
-      <c r="P95" s="11"/>
-      <c r="Q95" s="11"/>
-      <c r="R95" s="11"/>
-      <c r="S95" s="11"/>
       <c r="T95" s="5"/>
     </row>
     <row r="96" spans="1:20">
       <c r="A96" s="4"/>
-      <c r="B96" s="11"/>
-      <c r="C96" s="11"/>
-      <c r="D96" s="11"/>
-      <c r="E96" s="11"/>
-      <c r="F96" s="11"/>
-      <c r="G96" s="11"/>
-      <c r="H96" s="11"/>
-      <c r="I96" s="11"/>
-      <c r="J96" s="11"/>
-      <c r="K96" s="11"/>
-      <c r="L96" s="11"/>
-      <c r="M96" s="11"/>
-      <c r="N96" s="11"/>
-      <c r="O96" s="11"/>
-      <c r="P96" s="11"/>
-      <c r="Q96" s="11"/>
-      <c r="R96" s="11"/>
-      <c r="S96" s="11"/>
       <c r="T96" s="5"/>
     </row>
     <row r="97" spans="1:20">
       <c r="A97" s="4"/>
-      <c r="B97" s="11"/>
-      <c r="C97" s="11"/>
-      <c r="D97" s="11"/>
-      <c r="E97" s="11"/>
-      <c r="F97" s="11"/>
-      <c r="G97" s="11"/>
-      <c r="H97" s="11"/>
-      <c r="I97" s="11"/>
-      <c r="J97" s="11"/>
-      <c r="K97" s="11"/>
-      <c r="L97" s="11"/>
-      <c r="M97" s="11"/>
-      <c r="N97" s="11"/>
-      <c r="O97" s="11"/>
-      <c r="P97" s="11"/>
-      <c r="Q97" s="11"/>
-      <c r="R97" s="11"/>
-      <c r="S97" s="11"/>
       <c r="T97" s="5"/>
     </row>
     <row r="98" spans="1:20">
       <c r="A98" s="4"/>
-      <c r="B98" s="11"/>
-      <c r="C98" s="11"/>
-      <c r="D98" s="11"/>
-      <c r="E98" s="11"/>
-      <c r="F98" s="11"/>
-      <c r="G98" s="11"/>
-      <c r="H98" s="11"/>
-      <c r="I98" s="11"/>
-      <c r="J98" s="11"/>
-      <c r="K98" s="11"/>
-      <c r="L98" s="11"/>
-      <c r="M98" s="11"/>
-      <c r="N98" s="11"/>
-      <c r="O98" s="11"/>
-      <c r="P98" s="11"/>
-      <c r="Q98" s="11"/>
-      <c r="R98" s="11"/>
-      <c r="S98" s="11"/>
       <c r="T98" s="5"/>
     </row>
     <row r="99" spans="1:20">
       <c r="A99" s="4"/>
-      <c r="B99" s="11"/>
-      <c r="C99" s="11"/>
-      <c r="D99" s="11"/>
-      <c r="E99" s="11"/>
-      <c r="F99" s="11"/>
-      <c r="G99" s="11"/>
-      <c r="H99" s="11"/>
-      <c r="I99" s="11"/>
-      <c r="J99" s="11"/>
-      <c r="K99" s="11"/>
-      <c r="L99" s="11"/>
-      <c r="M99" s="11"/>
-      <c r="N99" s="11"/>
-      <c r="O99" s="11"/>
-      <c r="P99" s="11"/>
-      <c r="Q99" s="11"/>
-      <c r="R99" s="11"/>
-      <c r="S99" s="11"/>
       <c r="T99" s="5"/>
     </row>
     <row r="100" spans="1:20">
       <c r="A100" s="4"/>
-      <c r="B100" s="11"/>
-      <c r="C100" s="11"/>
-      <c r="D100" s="11"/>
-      <c r="E100" s="11"/>
-      <c r="F100" s="11"/>
-      <c r="G100" s="11"/>
-      <c r="H100" s="11"/>
-      <c r="I100" s="11"/>
-      <c r="J100" s="11"/>
-      <c r="K100" s="11"/>
-      <c r="L100" s="11"/>
-      <c r="M100" s="11"/>
-      <c r="N100" s="11"/>
-      <c r="O100" s="11"/>
-      <c r="P100" s="11"/>
-      <c r="Q100" s="11"/>
-      <c r="R100" s="11"/>
-      <c r="S100" s="11"/>
       <c r="T100" s="5"/>
     </row>
     <row r="101" spans="1:20">
       <c r="A101" s="4"/>
-      <c r="B101" s="11"/>
-      <c r="C101" s="11"/>
-      <c r="D101" s="11"/>
-      <c r="E101" s="11"/>
-      <c r="F101" s="11"/>
-      <c r="G101" s="11"/>
-      <c r="H101" s="11"/>
-      <c r="I101" s="11"/>
-      <c r="J101" s="11"/>
-      <c r="K101" s="11"/>
-      <c r="L101" s="11"/>
-      <c r="M101" s="11"/>
-      <c r="N101" s="11"/>
-      <c r="O101" s="11"/>
-      <c r="P101" s="11"/>
-      <c r="Q101" s="11"/>
-      <c r="R101" s="11"/>
-      <c r="S101" s="11"/>
       <c r="T101" s="5"/>
     </row>
     <row r="102" spans="1:20">
       <c r="A102" s="4"/>
-      <c r="B102" s="11"/>
-      <c r="C102" s="11"/>
-      <c r="D102" s="11"/>
-      <c r="E102" s="11"/>
-      <c r="F102" s="11"/>
-      <c r="G102" s="11"/>
-      <c r="H102" s="11"/>
-      <c r="I102" s="11"/>
-      <c r="J102" s="11"/>
-      <c r="K102" s="11"/>
-      <c r="L102" s="11"/>
-      <c r="M102" s="11"/>
-      <c r="N102" s="11"/>
-      <c r="O102" s="11"/>
-      <c r="P102" s="11"/>
-      <c r="Q102" s="11"/>
-      <c r="R102" s="11"/>
-      <c r="S102" s="11"/>
       <c r="T102" s="5"/>
     </row>
     <row r="103" spans="1:20">
       <c r="A103" s="4"/>
-      <c r="B103" s="11"/>
-      <c r="C103" s="11"/>
-      <c r="D103" s="11"/>
-      <c r="E103" s="11"/>
-      <c r="F103" s="11"/>
-      <c r="G103" s="11"/>
-      <c r="H103" s="11"/>
-      <c r="I103" s="11"/>
-      <c r="J103" s="11"/>
-      <c r="K103" s="11"/>
-      <c r="L103" s="11"/>
-      <c r="M103" s="11"/>
-      <c r="N103" s="11"/>
-      <c r="O103" s="11"/>
-      <c r="P103" s="11"/>
-      <c r="Q103" s="11"/>
-      <c r="R103" s="11"/>
-      <c r="S103" s="11"/>
       <c r="T103" s="5"/>
     </row>
     <row r="104" spans="1:20">
       <c r="A104" s="4"/>
-      <c r="B104" s="11"/>
-      <c r="C104" s="11"/>
-      <c r="D104" s="11"/>
-      <c r="E104" s="11"/>
-      <c r="F104" s="11"/>
-      <c r="G104" s="11"/>
-      <c r="H104" s="11"/>
-      <c r="I104" s="11"/>
-      <c r="J104" s="11"/>
-      <c r="K104" s="11"/>
-      <c r="L104" s="11"/>
-      <c r="M104" s="11"/>
-      <c r="N104" s="11"/>
-      <c r="O104" s="11"/>
-      <c r="P104" s="11"/>
-      <c r="Q104" s="11"/>
-      <c r="R104" s="11"/>
-      <c r="S104" s="11"/>
       <c r="T104" s="5"/>
     </row>
     <row r="105" spans="1:20">
       <c r="A105" s="4"/>
-      <c r="B105" s="11"/>
-      <c r="C105" s="11"/>
-      <c r="D105" s="11"/>
-      <c r="E105" s="11"/>
-      <c r="F105" s="11"/>
-      <c r="G105" s="11"/>
-      <c r="H105" s="11"/>
-      <c r="I105" s="11"/>
-      <c r="J105" s="11"/>
-      <c r="K105" s="11"/>
-      <c r="L105" s="11"/>
-      <c r="M105" s="11"/>
-      <c r="N105" s="11"/>
-      <c r="O105" s="11"/>
-      <c r="P105" s="11"/>
-      <c r="Q105" s="11"/>
-      <c r="R105" s="11"/>
-      <c r="S105" s="11"/>
       <c r="T105" s="5"/>
     </row>
     <row r="106" spans="1:20">
       <c r="A106" s="4"/>
-      <c r="B106" s="11"/>
-      <c r="C106" s="11"/>
-      <c r="D106" s="11"/>
-      <c r="E106" s="11"/>
-      <c r="F106" s="11"/>
-      <c r="G106" s="11"/>
-      <c r="H106" s="11"/>
-      <c r="I106" s="11"/>
-      <c r="J106" s="11"/>
-      <c r="K106" s="11"/>
-      <c r="L106" s="11"/>
-      <c r="M106" s="11"/>
-      <c r="N106" s="11"/>
-      <c r="O106" s="11"/>
-      <c r="P106" s="11"/>
-      <c r="Q106" s="11"/>
-      <c r="R106" s="11"/>
-      <c r="S106" s="11"/>
       <c r="T106" s="5"/>
     </row>
     <row r="107" spans="1:20">
       <c r="A107" s="4"/>
-      <c r="B107" s="11"/>
-      <c r="C107" s="11"/>
-      <c r="D107" s="11"/>
-      <c r="E107" s="11"/>
-      <c r="F107" s="11"/>
-      <c r="G107" s="11"/>
-      <c r="H107" s="11"/>
-      <c r="I107" s="11"/>
-      <c r="J107" s="11"/>
-      <c r="K107" s="11"/>
-      <c r="L107" s="11"/>
-      <c r="M107" s="11"/>
-      <c r="N107" s="11"/>
-      <c r="O107" s="11"/>
-      <c r="P107" s="11"/>
-      <c r="Q107" s="11"/>
-      <c r="R107" s="11"/>
-      <c r="S107" s="11"/>
       <c r="T107" s="5"/>
     </row>
     <row r="108" spans="1:20">
       <c r="A108" s="4"/>
-      <c r="B108" s="11"/>
-      <c r="C108" s="11"/>
-      <c r="D108" s="11"/>
-      <c r="E108" s="11"/>
-      <c r="F108" s="11"/>
-      <c r="G108" s="11"/>
-      <c r="H108" s="11"/>
-      <c r="I108" s="11"/>
-      <c r="J108" s="11"/>
-      <c r="K108" s="11"/>
-      <c r="L108" s="11"/>
-      <c r="M108" s="11"/>
-      <c r="N108" s="11"/>
-      <c r="O108" s="11"/>
-      <c r="P108" s="11"/>
-      <c r="Q108" s="11"/>
-      <c r="R108" s="11"/>
-      <c r="S108" s="11"/>
       <c r="T108" s="5"/>
     </row>
     <row r="109" spans="1:20">
       <c r="A109" s="4"/>
-      <c r="B109" s="11"/>
-      <c r="C109" s="11"/>
-      <c r="D109" s="11"/>
-      <c r="E109" s="11"/>
-      <c r="F109" s="11"/>
-      <c r="G109" s="11"/>
-      <c r="H109" s="11"/>
-      <c r="I109" s="11"/>
-      <c r="J109" s="11"/>
-      <c r="K109" s="11"/>
-      <c r="L109" s="11"/>
-      <c r="M109" s="11"/>
-      <c r="N109" s="11"/>
-      <c r="O109" s="11"/>
-      <c r="P109" s="11"/>
-      <c r="Q109" s="11"/>
-      <c r="R109" s="11"/>
-      <c r="S109" s="11"/>
       <c r="T109" s="5"/>
     </row>
     <row r="110" spans="1:20">
       <c r="A110" s="4"/>
-      <c r="B110" s="11"/>
-      <c r="C110" s="11"/>
-      <c r="D110" s="11"/>
-      <c r="E110" s="11"/>
-      <c r="F110" s="11"/>
-      <c r="G110" s="11"/>
-      <c r="H110" s="11"/>
-      <c r="I110" s="11"/>
-      <c r="J110" s="11"/>
-      <c r="K110" s="11"/>
-      <c r="L110" s="11"/>
-      <c r="M110" s="11"/>
-      <c r="N110" s="11"/>
-      <c r="O110" s="11"/>
-      <c r="P110" s="11"/>
-      <c r="Q110" s="11"/>
-      <c r="R110" s="11"/>
-      <c r="S110" s="11"/>
       <c r="T110" s="5"/>
     </row>
     <row r="111" spans="1:20">
       <c r="A111" s="4"/>
-      <c r="B111" s="11"/>
-      <c r="C111" s="11"/>
-      <c r="D111" s="11"/>
-      <c r="E111" s="11"/>
-      <c r="F111" s="11"/>
-      <c r="G111" s="11"/>
-      <c r="H111" s="11"/>
-      <c r="I111" s="11"/>
-      <c r="J111" s="11"/>
-      <c r="K111" s="11"/>
-      <c r="L111" s="11"/>
-      <c r="M111" s="11"/>
-      <c r="N111" s="11"/>
-      <c r="O111" s="11"/>
-      <c r="P111" s="11"/>
-      <c r="Q111" s="11"/>
-      <c r="R111" s="11"/>
-      <c r="S111" s="11"/>
       <c r="T111" s="5"/>
     </row>
     <row r="112" spans="1:20">
       <c r="A112" s="4"/>
-      <c r="B112" s="11"/>
-      <c r="C112" s="11"/>
-      <c r="D112" s="11"/>
-      <c r="E112" s="11"/>
-      <c r="F112" s="11"/>
-      <c r="G112" s="11"/>
-      <c r="H112" s="11"/>
-      <c r="I112" s="11"/>
-      <c r="J112" s="11"/>
-      <c r="K112" s="11"/>
-      <c r="L112" s="11"/>
-      <c r="M112" s="11"/>
-      <c r="N112" s="11"/>
-      <c r="O112" s="11"/>
-      <c r="P112" s="11"/>
-      <c r="Q112" s="11"/>
-      <c r="R112" s="11"/>
-      <c r="S112" s="11"/>
       <c r="T112" s="5"/>
     </row>
     <row r="113" spans="1:20">
       <c r="A113" s="4"/>
-      <c r="B113" s="11"/>
-      <c r="C113" s="11"/>
-      <c r="D113" s="11"/>
-      <c r="E113" s="11"/>
-      <c r="F113" s="11"/>
-      <c r="G113" s="11"/>
-      <c r="H113" s="11"/>
-      <c r="I113" s="11"/>
-      <c r="J113" s="11"/>
-      <c r="K113" s="11"/>
-      <c r="L113" s="11"/>
-      <c r="M113" s="11"/>
-      <c r="N113" s="11"/>
-      <c r="O113" s="11"/>
-      <c r="P113" s="11"/>
-      <c r="Q113" s="11"/>
-      <c r="R113" s="11"/>
-      <c r="S113" s="11"/>
       <c r="T113" s="5"/>
     </row>
     <row r="114" spans="1:20">
       <c r="A114" s="4"/>
-      <c r="B114" s="11"/>
-      <c r="C114" s="11"/>
-      <c r="D114" s="11"/>
-      <c r="E114" s="11"/>
-      <c r="F114" s="11"/>
-      <c r="G114" s="11"/>
-      <c r="H114" s="11"/>
-      <c r="I114" s="11"/>
-      <c r="J114" s="11"/>
-      <c r="K114" s="11"/>
-      <c r="L114" s="11"/>
-      <c r="M114" s="11"/>
-      <c r="N114" s="11"/>
-      <c r="O114" s="11"/>
-      <c r="P114" s="11"/>
-      <c r="Q114" s="11"/>
-      <c r="R114" s="11"/>
-      <c r="S114" s="11"/>
       <c r="T114" s="5"/>
     </row>
     <row r="115" spans="1:20">
       <c r="A115" s="4"/>
-      <c r="B115" s="11"/>
-      <c r="C115" s="11"/>
-      <c r="D115" s="11"/>
-      <c r="E115" s="11"/>
-      <c r="F115" s="11"/>
-      <c r="G115" s="11"/>
-      <c r="H115" s="11"/>
-      <c r="I115" s="11"/>
-      <c r="J115" s="11"/>
-      <c r="K115" s="11"/>
-      <c r="L115" s="11"/>
-      <c r="M115" s="11"/>
-      <c r="N115" s="11"/>
-      <c r="O115" s="11"/>
-      <c r="P115" s="11"/>
-      <c r="Q115" s="11"/>
-      <c r="R115" s="11"/>
-      <c r="S115" s="11"/>
       <c r="T115" s="5"/>
     </row>
     <row r="116" spans="1:20">
       <c r="A116" s="4"/>
-      <c r="B116" s="11"/>
-      <c r="C116" s="11"/>
-      <c r="D116" s="11"/>
-      <c r="E116" s="11"/>
-      <c r="F116" s="11"/>
-      <c r="G116" s="11"/>
-      <c r="H116" s="11"/>
-      <c r="I116" s="11"/>
-      <c r="J116" s="11"/>
-      <c r="K116" s="11"/>
-      <c r="L116" s="11"/>
-      <c r="M116" s="11"/>
-      <c r="N116" s="11"/>
-      <c r="O116" s="11"/>
-      <c r="P116" s="11"/>
-      <c r="Q116" s="11"/>
-      <c r="R116" s="11"/>
-      <c r="S116" s="11"/>
       <c r="T116" s="5"/>
     </row>
     <row r="117" spans="1:20">
       <c r="A117" s="4"/>
-      <c r="B117" s="11"/>
-      <c r="C117" s="11"/>
-      <c r="D117" s="11"/>
-      <c r="E117" s="11"/>
-      <c r="F117" s="11"/>
-      <c r="G117" s="11"/>
-      <c r="H117" s="11"/>
-      <c r="I117" s="11"/>
-      <c r="J117" s="11"/>
-      <c r="K117" s="11"/>
-      <c r="L117" s="11"/>
-      <c r="M117" s="11"/>
-      <c r="N117" s="11"/>
-      <c r="O117" s="11"/>
-      <c r="P117" s="11"/>
-      <c r="Q117" s="11"/>
-      <c r="R117" s="11"/>
-      <c r="S117" s="11"/>
       <c r="T117" s="5"/>
     </row>
     <row r="118" spans="1:20">
@@ -5006,4 +3978,228 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{817C6DA9-5F5B-4AE0-951D-8C0805A0232A}">
+  <dimension ref="A3:J87"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A39" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="U50" sqref="U50"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="18"/>
+  <sheetData>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" s="9" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="67" spans="3:10">
+      <c r="C67" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D67" s="2"/>
+      <c r="E67" s="2"/>
+      <c r="F67" s="2"/>
+      <c r="G67" s="2"/>
+      <c r="H67" s="2"/>
+      <c r="I67" s="2"/>
+      <c r="J67" s="3"/>
+    </row>
+    <row r="68" spans="3:10">
+      <c r="C68" s="4"/>
+      <c r="D68" s="11"/>
+      <c r="E68" s="11"/>
+      <c r="F68" s="11"/>
+      <c r="G68" s="11"/>
+      <c r="H68" s="11"/>
+      <c r="I68" s="11"/>
+      <c r="J68" s="5"/>
+    </row>
+    <row r="69" spans="3:10">
+      <c r="C69" s="4"/>
+      <c r="D69" s="11"/>
+      <c r="E69" s="11"/>
+      <c r="F69" s="11"/>
+      <c r="G69" s="11"/>
+      <c r="H69" s="11"/>
+      <c r="I69" s="11"/>
+      <c r="J69" s="5"/>
+    </row>
+    <row r="70" spans="3:10">
+      <c r="C70" s="4"/>
+      <c r="D70" s="11"/>
+      <c r="E70" s="11"/>
+      <c r="F70" s="11"/>
+      <c r="G70" s="11"/>
+      <c r="H70" s="11"/>
+      <c r="I70" s="11"/>
+      <c r="J70" s="5"/>
+    </row>
+    <row r="71" spans="3:10">
+      <c r="C71" s="4"/>
+      <c r="D71" s="11"/>
+      <c r="E71" s="11"/>
+      <c r="F71" s="11"/>
+      <c r="G71" s="11"/>
+      <c r="H71" s="11"/>
+      <c r="I71" s="11"/>
+      <c r="J71" s="5"/>
+    </row>
+    <row r="72" spans="3:10">
+      <c r="C72" s="4"/>
+      <c r="D72" s="11"/>
+      <c r="E72" s="11"/>
+      <c r="F72" s="11"/>
+      <c r="G72" s="11"/>
+      <c r="H72" s="11"/>
+      <c r="I72" s="11"/>
+      <c r="J72" s="5"/>
+    </row>
+    <row r="73" spans="3:10">
+      <c r="C73" s="4"/>
+      <c r="D73" s="11"/>
+      <c r="E73" s="11"/>
+      <c r="F73" s="11"/>
+      <c r="G73" s="11"/>
+      <c r="H73" s="11"/>
+      <c r="I73" s="11"/>
+      <c r="J73" s="5"/>
+    </row>
+    <row r="74" spans="3:10">
+      <c r="C74" s="4"/>
+      <c r="D74" s="11"/>
+      <c r="E74" s="11"/>
+      <c r="F74" s="11"/>
+      <c r="G74" s="11"/>
+      <c r="H74" s="11"/>
+      <c r="I74" s="11"/>
+      <c r="J74" s="5"/>
+    </row>
+    <row r="75" spans="3:10">
+      <c r="C75" s="4"/>
+      <c r="D75" s="11"/>
+      <c r="E75" s="11"/>
+      <c r="F75" s="11"/>
+      <c r="G75" s="11"/>
+      <c r="H75" s="11"/>
+      <c r="I75" s="11"/>
+      <c r="J75" s="5"/>
+    </row>
+    <row r="76" spans="3:10">
+      <c r="C76" s="4"/>
+      <c r="D76" s="11"/>
+      <c r="E76" s="11"/>
+      <c r="F76" s="11"/>
+      <c r="G76" s="11"/>
+      <c r="H76" s="11"/>
+      <c r="I76" s="11"/>
+      <c r="J76" s="5"/>
+    </row>
+    <row r="77" spans="3:10">
+      <c r="C77" s="4"/>
+      <c r="D77" s="11"/>
+      <c r="E77" s="11"/>
+      <c r="F77" s="11"/>
+      <c r="G77" s="11"/>
+      <c r="H77" s="11"/>
+      <c r="I77" s="11"/>
+      <c r="J77" s="5"/>
+    </row>
+    <row r="78" spans="3:10">
+      <c r="C78" s="6"/>
+      <c r="D78" s="7"/>
+      <c r="E78" s="7"/>
+      <c r="F78" s="7"/>
+      <c r="G78" s="7"/>
+      <c r="H78" s="7"/>
+      <c r="I78" s="7"/>
+      <c r="J78" s="8"/>
+    </row>
+    <row r="81" spans="3:9">
+      <c r="C81" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D81" s="2"/>
+      <c r="E81" s="2"/>
+      <c r="F81" s="2"/>
+      <c r="G81" s="2"/>
+      <c r="H81" s="2"/>
+      <c r="I81" s="3"/>
+    </row>
+    <row r="82" spans="3:9">
+      <c r="C82" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="D82" s="11"/>
+      <c r="E82" s="11"/>
+      <c r="F82" s="11"/>
+      <c r="G82" s="11"/>
+      <c r="H82" s="11"/>
+      <c r="I82" s="5"/>
+    </row>
+    <row r="83" spans="3:9">
+      <c r="C83" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="D83" s="11"/>
+      <c r="E83" s="11"/>
+      <c r="F83" s="11"/>
+      <c r="G83" s="11"/>
+      <c r="H83" s="11"/>
+      <c r="I83" s="5"/>
+    </row>
+    <row r="84" spans="3:9">
+      <c r="C84" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="D84" s="11"/>
+      <c r="E84" s="11"/>
+      <c r="F84" s="11"/>
+      <c r="G84" s="11"/>
+      <c r="H84" s="11"/>
+      <c r="I84" s="5"/>
+    </row>
+    <row r="85" spans="3:9">
+      <c r="C85" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="D85" s="11"/>
+      <c r="E85" s="11"/>
+      <c r="F85" s="11"/>
+      <c r="G85" s="11"/>
+      <c r="H85" s="11"/>
+      <c r="I85" s="5"/>
+    </row>
+    <row r="86" spans="3:9">
+      <c r="C86" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D86" s="11"/>
+      <c r="E86" s="11"/>
+      <c r="F86" s="11"/>
+      <c r="G86" s="11"/>
+      <c r="H86" s="11"/>
+      <c r="I86" s="5"/>
+    </row>
+    <row r="87" spans="3:9">
+      <c r="C87" s="6"/>
+      <c r="D87" s="7"/>
+      <c r="E87" s="7"/>
+      <c r="F87" s="7"/>
+      <c r="G87" s="7"/>
+      <c r="H87" s="7"/>
+      <c r="I87" s="8"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Input Data Using Forms
</commit_message>
<xml_diff>
--- a/3.VisualForce/1.Visualforce-Basics/1.Visualforce-Basics.xlsx
+++ b/3.VisualForce/1.Visualforce-Basics/1.Visualforce-Basics.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\quang\salesforce-trailhead\3.VisualForce\1.Visualforce-Basics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{606D40BA-65D2-470C-B2F7-A2BE9DEB8C1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{230A2702-8B9B-4290-A739-A6C2A7BEDF98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="3" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Create And Edit Visualforce Pag" sheetId="1" r:id="rId1"/>
     <sheet name="UseSimpleVariablesAndFormulas" sheetId="2" r:id="rId2"/>
     <sheet name="Use Standard Controllers" sheetId="3" r:id="rId3"/>
     <sheet name="DisplayRecordsFieldsAndTables" sheetId="4" r:id="rId4"/>
+    <sheet name="Input Data Using Forms" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="64">
   <si>
     <t>DisplayImage</t>
     <phoneticPr fontId="1"/>
@@ -248,6 +249,77 @@
         <scheme val="minor"/>
       </rPr>
       <t>name="OppView" standardController="Opportunity"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Input Data Using Forms</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>https://trailhead.salesforce.com/content/learn/modules/visualforce_fundamentals/visualforce_forms</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">    &lt;apex:form&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        &lt;apex:pageBlock title="Edit Contact"&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            &lt;apex:pageBlockSection&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                &lt;apex:inputField value="{! Contact.FirstName }"/&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                &lt;apex:inputField value="{! Contact.LastName }"/&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                &lt;apex:inputField value="{! Contact.Email }"/&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            &lt;/apex:pageBlockSection&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            &lt;apex:pageBlockButtons&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                &lt;apex:commandButton action="{! save }" value="Save" /&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            &lt;/apex:pageBlockButtons&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        &lt;/apex:pageBlock&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    &lt;/apex:form&gt;</t>
+  </si>
+  <si>
+    <r>
+      <t>&lt;apex:page</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Yu Gothic"/>
+        <family val="3"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> standardController="Contact"</t>
     </r>
     <r>
       <rPr>
@@ -415,9 +487,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
@@ -1731,6 +1803,319 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>127001</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>81644</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>111968</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="図 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E682373C-6380-1C64-E5A9-CB6AEC9BDABB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="789215" y="1021443"/>
+          <a:ext cx="11874500" cy="5667311"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>199571</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>163286</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>108285</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>51381</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="図 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A6FC09B6-8765-8AB7-1FAC-E87A72A1478A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="861785" y="6966857"/>
+          <a:ext cx="11828571" cy="6238095"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>235857</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>108857</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>47976</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>115404</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="図 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6E392A5A-07F2-DBAB-1C7C-3756C9FADBB5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="898071" y="13489214"/>
+          <a:ext cx="4447619" cy="2047619"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>453572</xdr:colOff>
+      <xdr:row>85</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>552762</xdr:colOff>
+      <xdr:row>112</xdr:row>
+      <xdr:rowOff>200595</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="図 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{33ADD573-2DD3-49A6-7589-25A468FC30DA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1115786" y="19276786"/>
+          <a:ext cx="12019047" cy="6323809"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>357085</xdr:colOff>
+      <xdr:row>113</xdr:row>
+      <xdr:rowOff>163285</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>161637</xdr:colOff>
+      <xdr:row>124</xdr:row>
+      <xdr:rowOff>116881</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="図 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{830032C6-AA36-ED53-F8DB-28CF479CBED8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1015176" y="26256012"/>
+          <a:ext cx="11650188" cy="2493596"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>134470</xdr:colOff>
+      <xdr:row>125</xdr:row>
+      <xdr:rowOff>104590</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>156791</xdr:colOff>
+      <xdr:row>148</xdr:row>
+      <xdr:rowOff>57729</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="図 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BFA322F4-6ADD-971F-DE6A-143AB314BE6B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="792561" y="28968226"/>
+          <a:ext cx="11867957" cy="5264048"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>207818</xdr:colOff>
+      <xdr:row>149</xdr:row>
+      <xdr:rowOff>150091</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>427182</xdr:colOff>
+      <xdr:row>172</xdr:row>
+      <xdr:rowOff>61065</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="図 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8A16FF68-60B9-C7AA-3D2E-79E8CEF9D70A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="865909" y="34555546"/>
+          <a:ext cx="12065000" cy="5221883"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -2122,7 +2507,7 @@
     </row>
     <row r="79" spans="2:20">
       <c r="B79" s="4"/>
-      <c r="C79" s="12" t="s">
+      <c r="C79" s="11" t="s">
         <v>2</v>
       </c>
       <c r="L79" s="5"/>
@@ -2286,7 +2671,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB076EE8-D0D3-4954-9948-E4CD27EFD4B6}">
   <dimension ref="A3:U242"/>
   <sheetViews>
-    <sheetView topLeftCell="A194" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+    <sheetView topLeftCell="A206" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <selection activeCell="AA220" sqref="AA219:AA220"/>
     </sheetView>
   </sheetViews>
@@ -3357,7 +3742,7 @@
     </row>
     <row r="213" spans="1:20">
       <c r="A213" s="4"/>
-      <c r="C213" s="12" t="s">
+      <c r="C213" s="11" t="s">
         <v>30</v>
       </c>
       <c r="E213" s="5"/>
@@ -3779,7 +4164,7 @@
     </row>
     <row r="84" spans="1:20">
       <c r="A84" s="4"/>
-      <c r="C84" s="12" t="s">
+      <c r="C84" s="11" t="s">
         <v>34</v>
       </c>
       <c r="H84" s="5"/>
@@ -3787,7 +4172,7 @@
     </row>
     <row r="85" spans="1:20">
       <c r="A85" s="4"/>
-      <c r="C85" s="13" t="s">
+      <c r="C85" s="12" t="s">
         <v>35</v>
       </c>
       <c r="H85" s="5"/>
@@ -3795,7 +4180,7 @@
     </row>
     <row r="86" spans="1:20">
       <c r="A86" s="4"/>
-      <c r="C86" s="13" t="s">
+      <c r="C86" s="12" t="s">
         <v>36</v>
       </c>
       <c r="H86" s="5"/>
@@ -3803,7 +4188,7 @@
     </row>
     <row r="87" spans="1:20">
       <c r="A87" s="4"/>
-      <c r="C87" s="13" t="s">
+      <c r="C87" s="12" t="s">
         <v>37</v>
       </c>
       <c r="H87" s="5"/>
@@ -3811,7 +4196,7 @@
     </row>
     <row r="88" spans="1:20">
       <c r="A88" s="4"/>
-      <c r="C88" s="13" t="s">
+      <c r="C88" s="12" t="s">
         <v>38</v>
       </c>
       <c r="H88" s="5"/>
@@ -3819,7 +4204,7 @@
     </row>
     <row r="89" spans="1:20">
       <c r="A89" s="4"/>
-      <c r="C89" s="13" t="s">
+      <c r="C89" s="12" t="s">
         <v>26</v>
       </c>
       <c r="H89" s="5"/>
@@ -3827,7 +4212,7 @@
     </row>
     <row r="90" spans="1:20">
       <c r="A90" s="4"/>
-      <c r="C90" s="13" t="s">
+      <c r="C90" s="12" t="s">
         <v>27</v>
       </c>
       <c r="H90" s="5"/>
@@ -3984,7 +4369,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{817C6DA9-5F5B-4AE0-951D-8C0805A0232A}">
   <dimension ref="A3:J87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="A76" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="U50" sqref="U50"/>
     </sheetView>
   </sheetViews>
@@ -4014,102 +4399,42 @@
     </row>
     <row r="68" spans="3:10">
       <c r="C68" s="4"/>
-      <c r="D68" s="11"/>
-      <c r="E68" s="11"/>
-      <c r="F68" s="11"/>
-      <c r="G68" s="11"/>
-      <c r="H68" s="11"/>
-      <c r="I68" s="11"/>
       <c r="J68" s="5"/>
     </row>
     <row r="69" spans="3:10">
       <c r="C69" s="4"/>
-      <c r="D69" s="11"/>
-      <c r="E69" s="11"/>
-      <c r="F69" s="11"/>
-      <c r="G69" s="11"/>
-      <c r="H69" s="11"/>
-      <c r="I69" s="11"/>
       <c r="J69" s="5"/>
     </row>
     <row r="70" spans="3:10">
       <c r="C70" s="4"/>
-      <c r="D70" s="11"/>
-      <c r="E70" s="11"/>
-      <c r="F70" s="11"/>
-      <c r="G70" s="11"/>
-      <c r="H70" s="11"/>
-      <c r="I70" s="11"/>
       <c r="J70" s="5"/>
     </row>
     <row r="71" spans="3:10">
       <c r="C71" s="4"/>
-      <c r="D71" s="11"/>
-      <c r="E71" s="11"/>
-      <c r="F71" s="11"/>
-      <c r="G71" s="11"/>
-      <c r="H71" s="11"/>
-      <c r="I71" s="11"/>
       <c r="J71" s="5"/>
     </row>
     <row r="72" spans="3:10">
       <c r="C72" s="4"/>
-      <c r="D72" s="11"/>
-      <c r="E72" s="11"/>
-      <c r="F72" s="11"/>
-      <c r="G72" s="11"/>
-      <c r="H72" s="11"/>
-      <c r="I72" s="11"/>
       <c r="J72" s="5"/>
     </row>
     <row r="73" spans="3:10">
       <c r="C73" s="4"/>
-      <c r="D73" s="11"/>
-      <c r="E73" s="11"/>
-      <c r="F73" s="11"/>
-      <c r="G73" s="11"/>
-      <c r="H73" s="11"/>
-      <c r="I73" s="11"/>
       <c r="J73" s="5"/>
     </row>
     <row r="74" spans="3:10">
       <c r="C74" s="4"/>
-      <c r="D74" s="11"/>
-      <c r="E74" s="11"/>
-      <c r="F74" s="11"/>
-      <c r="G74" s="11"/>
-      <c r="H74" s="11"/>
-      <c r="I74" s="11"/>
       <c r="J74" s="5"/>
     </row>
     <row r="75" spans="3:10">
       <c r="C75" s="4"/>
-      <c r="D75" s="11"/>
-      <c r="E75" s="11"/>
-      <c r="F75" s="11"/>
-      <c r="G75" s="11"/>
-      <c r="H75" s="11"/>
-      <c r="I75" s="11"/>
       <c r="J75" s="5"/>
     </row>
     <row r="76" spans="3:10">
       <c r="C76" s="4"/>
-      <c r="D76" s="11"/>
-      <c r="E76" s="11"/>
-      <c r="F76" s="11"/>
-      <c r="G76" s="11"/>
-      <c r="H76" s="11"/>
-      <c r="I76" s="11"/>
       <c r="J76" s="5"/>
     </row>
     <row r="77" spans="3:10">
       <c r="C77" s="4"/>
-      <c r="D77" s="11"/>
-      <c r="E77" s="11"/>
-      <c r="F77" s="11"/>
-      <c r="G77" s="11"/>
-      <c r="H77" s="11"/>
-      <c r="I77" s="11"/>
       <c r="J77" s="5"/>
     </row>
     <row r="78" spans="3:10">
@@ -4134,58 +4459,33 @@
       <c r="I81" s="3"/>
     </row>
     <row r="82" spans="3:9">
-      <c r="C82" s="12" t="s">
+      <c r="C82" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="D82" s="11"/>
-      <c r="E82" s="11"/>
-      <c r="F82" s="11"/>
-      <c r="G82" s="11"/>
-      <c r="H82" s="11"/>
       <c r="I82" s="5"/>
     </row>
     <row r="83" spans="3:9">
-      <c r="C83" s="13" t="s">
+      <c r="C83" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="D83" s="11"/>
-      <c r="E83" s="11"/>
-      <c r="F83" s="11"/>
-      <c r="G83" s="11"/>
-      <c r="H83" s="11"/>
       <c r="I83" s="5"/>
     </row>
     <row r="84" spans="3:9">
-      <c r="C84" s="13" t="s">
+      <c r="C84" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="D84" s="11"/>
-      <c r="E84" s="11"/>
-      <c r="F84" s="11"/>
-      <c r="G84" s="11"/>
-      <c r="H84" s="11"/>
       <c r="I84" s="5"/>
     </row>
     <row r="85" spans="3:9">
-      <c r="C85" s="13" t="s">
+      <c r="C85" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="D85" s="11"/>
-      <c r="E85" s="11"/>
-      <c r="F85" s="11"/>
-      <c r="G85" s="11"/>
-      <c r="H85" s="11"/>
       <c r="I85" s="5"/>
     </row>
     <row r="86" spans="3:9">
       <c r="C86" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D86" s="11"/>
-      <c r="E86" s="11"/>
-      <c r="F86" s="11"/>
-      <c r="G86" s="11"/>
-      <c r="H86" s="11"/>
       <c r="I86" s="5"/>
     </row>
     <row r="87" spans="3:9">
@@ -4202,4 +4502,185 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{972B7EAC-873F-4101-BC0B-AD7B6648777D}">
+  <dimension ref="A3:I84"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A87" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="X102" sqref="X102"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="18"/>
+  <sheetData>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" s="9" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="71" spans="3:9">
+      <c r="C71" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D71" s="2"/>
+      <c r="E71" s="2"/>
+      <c r="F71" s="2"/>
+      <c r="G71" s="2"/>
+      <c r="H71" s="2"/>
+      <c r="I71" s="3"/>
+    </row>
+    <row r="72" spans="3:9">
+      <c r="C72" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="D72" s="13"/>
+      <c r="E72" s="13"/>
+      <c r="F72" s="13"/>
+      <c r="G72" s="13"/>
+      <c r="H72" s="13"/>
+      <c r="I72" s="5"/>
+    </row>
+    <row r="73" spans="3:9">
+      <c r="C73" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="D73" s="13"/>
+      <c r="E73" s="13"/>
+      <c r="F73" s="13"/>
+      <c r="G73" s="13"/>
+      <c r="H73" s="13"/>
+      <c r="I73" s="5"/>
+    </row>
+    <row r="74" spans="3:9">
+      <c r="C74" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="D74" s="13"/>
+      <c r="E74" s="13"/>
+      <c r="F74" s="13"/>
+      <c r="G74" s="13"/>
+      <c r="H74" s="13"/>
+      <c r="I74" s="5"/>
+    </row>
+    <row r="75" spans="3:9">
+      <c r="C75" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="D75" s="13"/>
+      <c r="E75" s="13"/>
+      <c r="F75" s="13"/>
+      <c r="G75" s="13"/>
+      <c r="H75" s="13"/>
+      <c r="I75" s="5"/>
+    </row>
+    <row r="76" spans="3:9">
+      <c r="C76" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="D76" s="13"/>
+      <c r="E76" s="13"/>
+      <c r="F76" s="13"/>
+      <c r="G76" s="13"/>
+      <c r="H76" s="13"/>
+      <c r="I76" s="5"/>
+    </row>
+    <row r="77" spans="3:9">
+      <c r="C77" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="D77" s="13"/>
+      <c r="E77" s="13"/>
+      <c r="F77" s="13"/>
+      <c r="G77" s="13"/>
+      <c r="H77" s="13"/>
+      <c r="I77" s="5"/>
+    </row>
+    <row r="78" spans="3:9">
+      <c r="C78" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="D78" s="13"/>
+      <c r="E78" s="13"/>
+      <c r="F78" s="13"/>
+      <c r="G78" s="13"/>
+      <c r="H78" s="13"/>
+      <c r="I78" s="5"/>
+    </row>
+    <row r="79" spans="3:9">
+      <c r="C79" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="D79" s="13"/>
+      <c r="E79" s="13"/>
+      <c r="F79" s="13"/>
+      <c r="G79" s="13"/>
+      <c r="H79" s="13"/>
+      <c r="I79" s="5"/>
+    </row>
+    <row r="80" spans="3:9">
+      <c r="C80" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="D80" s="13"/>
+      <c r="E80" s="13"/>
+      <c r="F80" s="13"/>
+      <c r="G80" s="13"/>
+      <c r="H80" s="13"/>
+      <c r="I80" s="5"/>
+    </row>
+    <row r="81" spans="3:9">
+      <c r="C81" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="D81" s="13"/>
+      <c r="E81" s="13"/>
+      <c r="F81" s="13"/>
+      <c r="G81" s="13"/>
+      <c r="H81" s="13"/>
+      <c r="I81" s="5"/>
+    </row>
+    <row r="82" spans="3:9">
+      <c r="C82" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="D82" s="13"/>
+      <c r="E82" s="13"/>
+      <c r="F82" s="13"/>
+      <c r="G82" s="13"/>
+      <c r="H82" s="13"/>
+      <c r="I82" s="5"/>
+    </row>
+    <row r="83" spans="3:9">
+      <c r="C83" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="D83" s="13"/>
+      <c r="E83" s="13"/>
+      <c r="F83" s="13"/>
+      <c r="G83" s="13"/>
+      <c r="H83" s="13"/>
+      <c r="I83" s="5"/>
+    </row>
+    <row r="84" spans="3:9">
+      <c r="C84" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D84" s="7"/>
+      <c r="E84" s="7"/>
+      <c r="F84" s="7"/>
+      <c r="G84" s="7"/>
+      <c r="H84" s="7"/>
+      <c r="I84" s="8"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Use Standard List Controllers
</commit_message>
<xml_diff>
--- a/3.VisualForce/1.Visualforce-Basics/1.Visualforce-Basics.xlsx
+++ b/3.VisualForce/1.Visualforce-Basics/1.Visualforce-Basics.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\quang\salesforce-trailhead\3.VisualForce\1.Visualforce-Basics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{230A2702-8B9B-4290-A739-A6C2A7BEDF98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99DB1780-1DCD-41B5-A5A2-377070340D94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="3" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="4" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Create And Edit Visualforce Pag" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="Use Standard Controllers" sheetId="3" r:id="rId3"/>
     <sheet name="DisplayRecordsFieldsAndTables" sheetId="4" r:id="rId4"/>
     <sheet name="Input Data Using Forms" sheetId="5" r:id="rId5"/>
+    <sheet name="Use Standard List Controllers" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="76">
   <si>
     <t>DisplayImage</t>
     <phoneticPr fontId="1"/>
@@ -320,6 +321,70 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> standardController="Contact"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Use Standard List Controllers</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>https://trailhead.salesforce.com/content/learn/modules/visualforce_fundamentals/visualforce_standard_list_controllers</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>AccountList</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>CreateContact</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">    &lt;apex:repeat var="a" value="{! accounts }"&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        &lt;li&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                &lt;apex:outputText value="{! a.Name }"&gt;&lt;/apex:outputText&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            &lt;/apex:outputLink&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        &lt;/li&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    &lt;/apex:repeat&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            &lt;apex:outputLink value="/{!a.Id}"&gt;</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">&lt;apex:page </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Yu Gothic"/>
+        <family val="3"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>standardController="Account" recordSetVar="accounts"</t>
     </r>
     <r>
       <rPr>
@@ -1895,16 +1960,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>235857</xdr:colOff>
-      <xdr:row>59</xdr:row>
-      <xdr:rowOff>108857</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>226784</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>99786</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>47976</xdr:colOff>
-      <xdr:row>68</xdr:row>
-      <xdr:rowOff>115404</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>38903</xdr:colOff>
+      <xdr:row>69</xdr:row>
+      <xdr:rowOff>106334</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1927,7 +1992,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="898071" y="13489214"/>
+          <a:off x="1551213" y="13706929"/>
           <a:ext cx="4447619" cy="2047619"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1941,14 +2006,14 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>453572</xdr:colOff>
-      <xdr:row>85</xdr:row>
+      <xdr:row>86</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
       <xdr:colOff>552762</xdr:colOff>
-      <xdr:row>112</xdr:row>
-      <xdr:rowOff>200595</xdr:rowOff>
+      <xdr:row>113</xdr:row>
+      <xdr:rowOff>200594</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1985,13 +2050,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>357085</xdr:colOff>
-      <xdr:row>113</xdr:row>
+      <xdr:row>114</xdr:row>
       <xdr:rowOff>163285</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
       <xdr:colOff>161637</xdr:colOff>
-      <xdr:row>124</xdr:row>
+      <xdr:row>125</xdr:row>
       <xdr:rowOff>116881</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2029,14 +2094,14 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>134470</xdr:colOff>
-      <xdr:row>125</xdr:row>
+      <xdr:row>126</xdr:row>
       <xdr:rowOff>104590</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
       <xdr:colOff>156791</xdr:colOff>
-      <xdr:row>148</xdr:row>
-      <xdr:rowOff>57729</xdr:rowOff>
+      <xdr:row>149</xdr:row>
+      <xdr:rowOff>57730</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2073,13 +2138,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>207818</xdr:colOff>
-      <xdr:row>149</xdr:row>
+      <xdr:row>150</xdr:row>
       <xdr:rowOff>150091</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
       <xdr:colOff>427182</xdr:colOff>
-      <xdr:row>172</xdr:row>
+      <xdr:row>173</xdr:row>
       <xdr:rowOff>61065</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2105,6 +2170,231 @@
         <a:xfrm>
           <a:off x="865909" y="34555546"/>
           <a:ext cx="12065000" cy="5221883"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>92364</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>72444</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="図 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{493A71E5-6822-7556-6C24-F5BA77B3CCFD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="753341" y="999836"/>
+          <a:ext cx="11842750" cy="5307153"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>186765</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>112058</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>210496</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>144890</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="図 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B350752E-E2B2-105B-BC5A-AFBBFE042AE8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="844177" y="6596529"/>
+          <a:ext cx="11857143" cy="6285714"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>224117</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>149411</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>374616</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>109719</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="図 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{08930A61-31A7-0E2B-71B4-9E795CE0F837}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1538941" y="13581529"/>
+          <a:ext cx="4752381" cy="2276190"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>156882</xdr:colOff>
+      <xdr:row>81</xdr:row>
+      <xdr:rowOff>89647</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>254000</xdr:colOff>
+      <xdr:row>111</xdr:row>
+      <xdr:rowOff>115623</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="図 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{34A24DA5-96DA-9D5F-728A-22B04C6AD80B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="814973" y="18793283"/>
+          <a:ext cx="11942754" cy="6953249"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>242455</xdr:colOff>
+      <xdr:row>112</xdr:row>
+      <xdr:rowOff>161637</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>427182</xdr:colOff>
+      <xdr:row>135</xdr:row>
+      <xdr:rowOff>115190</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="図 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{85928285-100B-D28B-57C5-65B7B8379B1E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="900546" y="26023455"/>
+          <a:ext cx="12030363" cy="5264462"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4369,7 +4659,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{817C6DA9-5F5B-4AE0-951D-8C0805A0232A}">
   <dimension ref="A3:J87"/>
   <sheetViews>
-    <sheetView topLeftCell="A76" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="A61" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="U50" sqref="U50"/>
     </sheetView>
   </sheetViews>
@@ -4506,10 +4796,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{972B7EAC-873F-4101-BC0B-AD7B6648777D}">
-  <dimension ref="A3:I84"/>
+  <dimension ref="A3:J85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A87" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="X102" sqref="X102"/>
+    <sheetView topLeftCell="A73" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="S67" sqref="S67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18"/>
@@ -4524,159 +4814,478 @@
         <v>50</v>
       </c>
     </row>
-    <row r="71" spans="3:9">
+    <row r="60" spans="3:10">
+      <c r="C60" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D60" s="2"/>
+      <c r="E60" s="2"/>
+      <c r="F60" s="2"/>
+      <c r="G60" s="2"/>
+      <c r="H60" s="2"/>
+      <c r="I60" s="2"/>
+      <c r="J60" s="3"/>
+    </row>
+    <row r="61" spans="3:10">
+      <c r="C61" s="4"/>
+      <c r="D61" s="13"/>
+      <c r="E61" s="13"/>
+      <c r="F61" s="13"/>
+      <c r="G61" s="13"/>
+      <c r="H61" s="13"/>
+      <c r="I61" s="13"/>
+      <c r="J61" s="5"/>
+    </row>
+    <row r="62" spans="3:10">
+      <c r="C62" s="4"/>
+      <c r="D62" s="13"/>
+      <c r="E62" s="13"/>
+      <c r="F62" s="13"/>
+      <c r="G62" s="13"/>
+      <c r="H62" s="13"/>
+      <c r="I62" s="13"/>
+      <c r="J62" s="5"/>
+    </row>
+    <row r="63" spans="3:10">
+      <c r="C63" s="4"/>
+      <c r="D63" s="13"/>
+      <c r="E63" s="13"/>
+      <c r="F63" s="13"/>
+      <c r="G63" s="13"/>
+      <c r="H63" s="13"/>
+      <c r="I63" s="13"/>
+      <c r="J63" s="5"/>
+    </row>
+    <row r="64" spans="3:10">
+      <c r="C64" s="4"/>
+      <c r="D64" s="13"/>
+      <c r="E64" s="13"/>
+      <c r="F64" s="13"/>
+      <c r="G64" s="13"/>
+      <c r="H64" s="13"/>
+      <c r="I64" s="13"/>
+      <c r="J64" s="5"/>
+    </row>
+    <row r="65" spans="3:10">
+      <c r="C65" s="4"/>
+      <c r="D65" s="13"/>
+      <c r="E65" s="13"/>
+      <c r="F65" s="13"/>
+      <c r="G65" s="13"/>
+      <c r="H65" s="13"/>
+      <c r="I65" s="13"/>
+      <c r="J65" s="5"/>
+    </row>
+    <row r="66" spans="3:10">
+      <c r="C66" s="4"/>
+      <c r="D66" s="13"/>
+      <c r="E66" s="13"/>
+      <c r="F66" s="13"/>
+      <c r="G66" s="13"/>
+      <c r="H66" s="13"/>
+      <c r="I66" s="13"/>
+      <c r="J66" s="5"/>
+    </row>
+    <row r="67" spans="3:10">
+      <c r="C67" s="4"/>
+      <c r="D67" s="13"/>
+      <c r="E67" s="13"/>
+      <c r="F67" s="13"/>
+      <c r="G67" s="13"/>
+      <c r="H67" s="13"/>
+      <c r="I67" s="13"/>
+      <c r="J67" s="5"/>
+    </row>
+    <row r="68" spans="3:10">
+      <c r="C68" s="4"/>
+      <c r="D68" s="13"/>
+      <c r="E68" s="13"/>
+      <c r="F68" s="13"/>
+      <c r="G68" s="13"/>
+      <c r="H68" s="13"/>
+      <c r="I68" s="13"/>
+      <c r="J68" s="5"/>
+    </row>
+    <row r="69" spans="3:10">
+      <c r="C69" s="4"/>
+      <c r="D69" s="13"/>
+      <c r="E69" s="13"/>
+      <c r="F69" s="13"/>
+      <c r="G69" s="13"/>
+      <c r="H69" s="13"/>
+      <c r="I69" s="13"/>
+      <c r="J69" s="5"/>
+    </row>
+    <row r="70" spans="3:10">
+      <c r="C70" s="6"/>
+      <c r="D70" s="7"/>
+      <c r="E70" s="7"/>
+      <c r="F70" s="7"/>
+      <c r="G70" s="7"/>
+      <c r="H70" s="7"/>
+      <c r="I70" s="7"/>
+      <c r="J70" s="8"/>
+    </row>
+    <row r="72" spans="3:10">
+      <c r="C72" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D72" s="2"/>
+      <c r="E72" s="2"/>
+      <c r="F72" s="2"/>
+      <c r="G72" s="2"/>
+      <c r="H72" s="2"/>
+      <c r="I72" s="3"/>
+    </row>
+    <row r="73" spans="3:10">
+      <c r="C73" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="I73" s="5"/>
+    </row>
+    <row r="74" spans="3:10">
+      <c r="C74" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="I74" s="5"/>
+    </row>
+    <row r="75" spans="3:10">
+      <c r="C75" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="I75" s="5"/>
+    </row>
+    <row r="76" spans="3:10">
+      <c r="C76" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="I76" s="5"/>
+    </row>
+    <row r="77" spans="3:10">
+      <c r="C77" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="I77" s="5"/>
+    </row>
+    <row r="78" spans="3:10">
+      <c r="C78" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="I78" s="5"/>
+    </row>
+    <row r="79" spans="3:10">
+      <c r="C79" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="I79" s="5"/>
+    </row>
+    <row r="80" spans="3:10">
+      <c r="C80" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="I80" s="5"/>
+    </row>
+    <row r="81" spans="3:9">
+      <c r="C81" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="I81" s="5"/>
+    </row>
+    <row r="82" spans="3:9">
+      <c r="C82" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="I82" s="5"/>
+    </row>
+    <row r="83" spans="3:9">
+      <c r="C83" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="I83" s="5"/>
+    </row>
+    <row r="84" spans="3:9">
+      <c r="C84" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="I84" s="5"/>
+    </row>
+    <row r="85" spans="3:9">
+      <c r="C85" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D85" s="7"/>
+      <c r="E85" s="7"/>
+      <c r="F85" s="7"/>
+      <c r="G85" s="7"/>
+      <c r="H85" s="7"/>
+      <c r="I85" s="8"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E078833-1582-4D08-806F-71CEC3EB9A8D}">
+  <dimension ref="A3:J80"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A112" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="W129" sqref="W129"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="18"/>
+  <sheetData>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" s="9" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="58" spans="3:10">
+      <c r="C58" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D58" s="2"/>
+      <c r="E58" s="2"/>
+      <c r="F58" s="2"/>
+      <c r="G58" s="2"/>
+      <c r="H58" s="2"/>
+      <c r="I58" s="2"/>
+      <c r="J58" s="3"/>
+    </row>
+    <row r="59" spans="3:10">
+      <c r="C59" s="4"/>
+      <c r="D59" s="13"/>
+      <c r="E59" s="13"/>
+      <c r="F59" s="13"/>
+      <c r="G59" s="13"/>
+      <c r="H59" s="13"/>
+      <c r="I59" s="13"/>
+      <c r="J59" s="5"/>
+    </row>
+    <row r="60" spans="3:10">
+      <c r="C60" s="4"/>
+      <c r="D60" s="13"/>
+      <c r="E60" s="13"/>
+      <c r="F60" s="13"/>
+      <c r="G60" s="13"/>
+      <c r="H60" s="13"/>
+      <c r="I60" s="13"/>
+      <c r="J60" s="5"/>
+    </row>
+    <row r="61" spans="3:10">
+      <c r="C61" s="4"/>
+      <c r="D61" s="13"/>
+      <c r="E61" s="13"/>
+      <c r="F61" s="13"/>
+      <c r="G61" s="13"/>
+      <c r="H61" s="13"/>
+      <c r="I61" s="13"/>
+      <c r="J61" s="5"/>
+    </row>
+    <row r="62" spans="3:10">
+      <c r="C62" s="4"/>
+      <c r="D62" s="13"/>
+      <c r="E62" s="13"/>
+      <c r="F62" s="13"/>
+      <c r="G62" s="13"/>
+      <c r="H62" s="13"/>
+      <c r="I62" s="13"/>
+      <c r="J62" s="5"/>
+    </row>
+    <row r="63" spans="3:10">
+      <c r="C63" s="4"/>
+      <c r="D63" s="13"/>
+      <c r="E63" s="13"/>
+      <c r="F63" s="13"/>
+      <c r="G63" s="13"/>
+      <c r="H63" s="13"/>
+      <c r="I63" s="13"/>
+      <c r="J63" s="5"/>
+    </row>
+    <row r="64" spans="3:10">
+      <c r="C64" s="4"/>
+      <c r="D64" s="13"/>
+      <c r="E64" s="13"/>
+      <c r="F64" s="13"/>
+      <c r="G64" s="13"/>
+      <c r="H64" s="13"/>
+      <c r="I64" s="13"/>
+      <c r="J64" s="5"/>
+    </row>
+    <row r="65" spans="3:10">
+      <c r="C65" s="4"/>
+      <c r="D65" s="13"/>
+      <c r="E65" s="13"/>
+      <c r="F65" s="13"/>
+      <c r="G65" s="13"/>
+      <c r="H65" s="13"/>
+      <c r="I65" s="13"/>
+      <c r="J65" s="5"/>
+    </row>
+    <row r="66" spans="3:10">
+      <c r="C66" s="4"/>
+      <c r="D66" s="13"/>
+      <c r="E66" s="13"/>
+      <c r="F66" s="13"/>
+      <c r="G66" s="13"/>
+      <c r="H66" s="13"/>
+      <c r="I66" s="13"/>
+      <c r="J66" s="5"/>
+    </row>
+    <row r="67" spans="3:10">
+      <c r="C67" s="4"/>
+      <c r="D67" s="13"/>
+      <c r="E67" s="13"/>
+      <c r="F67" s="13"/>
+      <c r="G67" s="13"/>
+      <c r="H67" s="13"/>
+      <c r="I67" s="13"/>
+      <c r="J67" s="5"/>
+    </row>
+    <row r="68" spans="3:10">
+      <c r="C68" s="4"/>
+      <c r="D68" s="13"/>
+      <c r="E68" s="13"/>
+      <c r="F68" s="13"/>
+      <c r="G68" s="13"/>
+      <c r="H68" s="13"/>
+      <c r="I68" s="13"/>
+      <c r="J68" s="5"/>
+    </row>
+    <row r="69" spans="3:10">
+      <c r="C69" s="6"/>
+      <c r="D69" s="7"/>
+      <c r="E69" s="7"/>
+      <c r="F69" s="7"/>
+      <c r="G69" s="7"/>
+      <c r="H69" s="7"/>
+      <c r="I69" s="7"/>
+      <c r="J69" s="8"/>
+    </row>
+    <row r="71" spans="3:10">
       <c r="C71" s="1" t="s">
-        <v>63</v>
+        <v>75</v>
       </c>
       <c r="D71" s="2"/>
       <c r="E71" s="2"/>
       <c r="F71" s="2"/>
       <c r="G71" s="2"/>
       <c r="H71" s="2"/>
-      <c r="I71" s="3"/>
-    </row>
-    <row r="72" spans="3:9">
+      <c r="I71" s="2"/>
+      <c r="J71" s="3"/>
+    </row>
+    <row r="72" spans="3:10">
       <c r="C72" s="11" t="s">
-        <v>51</v>
+        <v>68</v>
       </c>
       <c r="D72" s="13"/>
       <c r="E72" s="13"/>
       <c r="F72" s="13"/>
       <c r="G72" s="13"/>
       <c r="H72" s="13"/>
-      <c r="I72" s="5"/>
-    </row>
-    <row r="73" spans="3:9">
+      <c r="I72" s="13"/>
+      <c r="J72" s="5"/>
+    </row>
+    <row r="73" spans="3:10">
       <c r="C73" s="12" t="s">
-        <v>52</v>
+        <v>69</v>
       </c>
       <c r="D73" s="13"/>
       <c r="E73" s="13"/>
       <c r="F73" s="13"/>
       <c r="G73" s="13"/>
       <c r="H73" s="13"/>
-      <c r="I73" s="5"/>
-    </row>
-    <row r="74" spans="3:9">
+      <c r="I73" s="13"/>
+      <c r="J73" s="5"/>
+    </row>
+    <row r="74" spans="3:10">
       <c r="C74" s="12" t="s">
-        <v>53</v>
+        <v>74</v>
       </c>
       <c r="D74" s="13"/>
       <c r="E74" s="13"/>
       <c r="F74" s="13"/>
       <c r="G74" s="13"/>
       <c r="H74" s="13"/>
-      <c r="I74" s="5"/>
-    </row>
-    <row r="75" spans="3:9">
+      <c r="I74" s="13"/>
+      <c r="J74" s="5"/>
+    </row>
+    <row r="75" spans="3:10">
       <c r="C75" s="12" t="s">
-        <v>54</v>
+        <v>70</v>
       </c>
       <c r="D75" s="13"/>
       <c r="E75" s="13"/>
       <c r="F75" s="13"/>
       <c r="G75" s="13"/>
       <c r="H75" s="13"/>
-      <c r="I75" s="5"/>
-    </row>
-    <row r="76" spans="3:9">
+      <c r="I75" s="13"/>
+      <c r="J75" s="5"/>
+    </row>
+    <row r="76" spans="3:10">
       <c r="C76" s="12" t="s">
-        <v>55</v>
+        <v>71</v>
       </c>
       <c r="D76" s="13"/>
       <c r="E76" s="13"/>
       <c r="F76" s="13"/>
       <c r="G76" s="13"/>
       <c r="H76" s="13"/>
-      <c r="I76" s="5"/>
-    </row>
-    <row r="77" spans="3:9">
+      <c r="I76" s="13"/>
+      <c r="J76" s="5"/>
+    </row>
+    <row r="77" spans="3:10">
       <c r="C77" s="12" t="s">
-        <v>56</v>
+        <v>72</v>
       </c>
       <c r="D77" s="13"/>
       <c r="E77" s="13"/>
       <c r="F77" s="13"/>
       <c r="G77" s="13"/>
       <c r="H77" s="13"/>
-      <c r="I77" s="5"/>
-    </row>
-    <row r="78" spans="3:9">
+      <c r="I77" s="13"/>
+      <c r="J77" s="5"/>
+    </row>
+    <row r="78" spans="3:10">
       <c r="C78" s="12" t="s">
-        <v>57</v>
+        <v>73</v>
       </c>
       <c r="D78" s="13"/>
       <c r="E78" s="13"/>
       <c r="F78" s="13"/>
       <c r="G78" s="13"/>
       <c r="H78" s="13"/>
-      <c r="I78" s="5"/>
-    </row>
-    <row r="79" spans="3:9">
-      <c r="C79" s="12" t="s">
-        <v>58</v>
+      <c r="I78" s="13"/>
+      <c r="J78" s="5"/>
+    </row>
+    <row r="79" spans="3:10">
+      <c r="C79" s="4" t="s">
+        <v>1</v>
       </c>
       <c r="D79" s="13"/>
       <c r="E79" s="13"/>
       <c r="F79" s="13"/>
       <c r="G79" s="13"/>
       <c r="H79" s="13"/>
-      <c r="I79" s="5"/>
-    </row>
-    <row r="80" spans="3:9">
-      <c r="C80" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="D80" s="13"/>
-      <c r="E80" s="13"/>
-      <c r="F80" s="13"/>
-      <c r="G80" s="13"/>
-      <c r="H80" s="13"/>
-      <c r="I80" s="5"/>
-    </row>
-    <row r="81" spans="3:9">
-      <c r="C81" s="12" t="s">
-        <v>60</v>
-      </c>
-      <c r="D81" s="13"/>
-      <c r="E81" s="13"/>
-      <c r="F81" s="13"/>
-      <c r="G81" s="13"/>
-      <c r="H81" s="13"/>
-      <c r="I81" s="5"/>
-    </row>
-    <row r="82" spans="3:9">
-      <c r="C82" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="D82" s="13"/>
-      <c r="E82" s="13"/>
-      <c r="F82" s="13"/>
-      <c r="G82" s="13"/>
-      <c r="H82" s="13"/>
-      <c r="I82" s="5"/>
-    </row>
-    <row r="83" spans="3:9">
-      <c r="C83" s="12" t="s">
-        <v>62</v>
-      </c>
-      <c r="D83" s="13"/>
-      <c r="E83" s="13"/>
-      <c r="F83" s="13"/>
-      <c r="G83" s="13"/>
-      <c r="H83" s="13"/>
-      <c r="I83" s="5"/>
-    </row>
-    <row r="84" spans="3:9">
-      <c r="C84" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="D84" s="7"/>
-      <c r="E84" s="7"/>
-      <c r="F84" s="7"/>
-      <c r="G84" s="7"/>
-      <c r="H84" s="7"/>
-      <c r="I84" s="8"/>
+      <c r="I79" s="13"/>
+      <c r="J79" s="5"/>
+    </row>
+    <row r="80" spans="3:10">
+      <c r="C80" s="6"/>
+      <c r="D80" s="7"/>
+      <c r="E80" s="7"/>
+      <c r="F80" s="7"/>
+      <c r="G80" s="7"/>
+      <c r="H80" s="7"/>
+      <c r="I80" s="7"/>
+      <c r="J80" s="8"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>

</xml_diff>